<commit_message>
Cleaned up terms, added some for PARADISEC
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="307">
   <si>
     <t>Name</t>
   </si>
@@ -82,22 +82,13 @@
     <t>sameAs</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>olac:Analysis</t>
+    <t>olac:Annotation</t>
   </si>
   <si>
     <t>DefinedTerm</t>
   </si>
   <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#Lexicon/analytical</t>
-  </si>
-  <si>
-    <t>olac:Annotation</t>
+    <t>The resource includes information which annotates some other linguistic record.</t>
   </si>
   <si>
     <t>Annotation</t>
@@ -109,165 +100,218 @@
     <t>olac:BornDigital</t>
   </si>
   <si>
+    <t>CommunicationModeValues</t>
+  </si>
+  <si>
     <t>BornDigital</t>
   </si>
   <si>
-    <t>CommunicationModeValues</t>
-  </si>
-  <si>
     <t>olac:Code</t>
   </si>
   <si>
+    <t>The resource contains a coded analysis or annotation</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
+    <t>olac:DerivedText</t>
+  </si>
+  <si>
+    <t>ResourceTypeValues</t>
+  </si>
+  <si>
+    <t>DerivedText</t>
+  </si>
+  <si>
+    <t>olac:Dialogue</t>
+  </si>
+  <si>
+    <t>CommunicationGenreValues</t>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t>olac:Gesture</t>
+  </si>
+  <si>
+    <t>Gesture</t>
+  </si>
+  <si>
+    <t>olac:Handwritten</t>
+  </si>
+  <si>
+    <t>The resource was written using a writing implement such as pen, pencil, brush or computer stylus</t>
+  </si>
+  <si>
+    <t>Handwritten</t>
+  </si>
+  <si>
+    <t>olac:Interview</t>
+  </si>
+  <si>
+    <t>The resource is conversation where one or more speakers are directing the conversation</t>
+  </si>
+  <si>
+    <t>Interview</t>
+  </si>
+  <si>
+    <t>olac:Lexicon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The resource includes a systematic listing of lexical items.
+</t>
+  </si>
+  <si>
+    <t>Lexicon</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#Lexicon</t>
+  </si>
+  <si>
+    <t>olac:LinguisticDescription</t>
+  </si>
+  <si>
+    <t>LinguisticDescription</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description</t>
+  </si>
+  <si>
+    <t>olac:Ludic</t>
+  </si>
+  <si>
+    <t>Ludic</t>
+  </si>
+  <si>
+    <t>olac:Narrative</t>
+  </si>
+  <si>
+    <t>A monologic discourse which represents temporally organized events.</t>
+  </si>
+  <si>
+    <t>Narrative</t>
+  </si>
+  <si>
+    <t>olac:NonDigital</t>
+  </si>
+  <si>
+    <t>The resource was not originally captured or created  in digital form</t>
+  </si>
+  <si>
+    <t>NonDigital</t>
+  </si>
+  <si>
+    <t>olac:NotBornDigital</t>
+  </si>
+  <si>
+    <t>NotBornDigital</t>
+  </si>
+  <si>
+    <t>olac:Oratory</t>
+  </si>
+  <si>
+    <t>Oratory</t>
+  </si>
+  <si>
+    <t>olac:Orthography</t>
+  </si>
+  <si>
+    <t>The resource contains written material using a standard or conventional orthography with conventions for punctuation, capitalization etc</t>
+  </si>
+  <si>
+    <t>Orthography</t>
+  </si>
+  <si>
+    <t>olac:PartOfSpeech</t>
+  </si>
+  <si>
+    <t>PartOfSpeech</t>
+  </si>
+  <si>
+    <t>olac:Phonemic</t>
+  </si>
+  <si>
+    <t>Phonemic</t>
+  </si>
+  <si>
+    <t>olac:Phonetic</t>
+  </si>
+  <si>
+    <t>Phonetic</t>
+  </si>
+  <si>
+    <t>olac:Phonological</t>
+  </si>
+  <si>
+    <t>Phonological</t>
+  </si>
+  <si>
+    <t>olac:PrimaryText</t>
+  </si>
+  <si>
+    <t>This is a primary resource: the object of study.   A text is defined as any primary resource or research material, such as a literary work, film, or recording of natural discourse</t>
+  </si>
+  <si>
+    <t>PrimaryText</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text</t>
+  </si>
+  <si>
+    <t>olac:Procedural</t>
+  </si>
+  <si>
+    <t>Procedural</t>
+  </si>
+  <si>
+    <t>olac:Prosodic</t>
+  </si>
+  <si>
+    <t>Prosodic</t>
+  </si>
+  <si>
+    <t>olac:Report</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>olac:Singing</t>
+  </si>
+  <si>
     <t>"Words or sounds [articulated] in succession with musical inflections or modulations of the voice" OED.</t>
   </si>
   <si>
-    <t>olac:DerivedText</t>
-  </si>
-  <si>
-    <t>DerivedText</t>
-  </si>
-  <si>
-    <t>ResourceTypeValues</t>
-  </si>
-  <si>
-    <t>olac:Dialogue</t>
-  </si>
-  <si>
-    <t>Dialogue</t>
-  </si>
-  <si>
-    <t>CommunicationGenreValues</t>
-  </si>
-  <si>
-    <t>olac:Gesture</t>
-  </si>
-  <si>
-    <t>Gesture</t>
-  </si>
-  <si>
-    <t>olac:Handwritten</t>
-  </si>
-  <si>
-    <t>Handwritten</t>
-  </si>
-  <si>
-    <t>olac:Interview</t>
-  </si>
-  <si>
-    <t>Interview</t>
-  </si>
-  <si>
-    <t>olac:Lexicon</t>
-  </si>
-  <si>
-    <t>Lexicon</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#Lexicon</t>
-  </si>
-  <si>
-    <t>olac:LinguisticDescription</t>
-  </si>
-  <si>
-    <t>LinguisticDescription</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#description</t>
-  </si>
-  <si>
-    <t>olac:Ludic</t>
-  </si>
-  <si>
-    <t>Ludic</t>
-  </si>
-  <si>
-    <t>olac:Narrative</t>
-  </si>
-  <si>
-    <t>Narrative</t>
-  </si>
-  <si>
-    <t>olac:NonDigital</t>
-  </si>
-  <si>
-    <t>NonDigital</t>
-  </si>
-  <si>
-    <t>olac:Oratory</t>
-  </si>
-  <si>
-    <t>Oratory</t>
-  </si>
-  <si>
-    <t>olac:Orthography</t>
-  </si>
-  <si>
-    <t>Orthography</t>
-  </si>
-  <si>
-    <t>olac:PartOfSpeech</t>
-  </si>
-  <si>
-    <t>PartOfSpeech</t>
-  </si>
-  <si>
-    <t>olac:Phonemic</t>
-  </si>
-  <si>
-    <t>Phonemic</t>
-  </si>
-  <si>
-    <t>olac:Phonetic</t>
-  </si>
-  <si>
-    <t>Phonetic</t>
-  </si>
-  <si>
-    <t>olac:Phonological</t>
-  </si>
-  <si>
-    <t>Phonological</t>
-  </si>
-  <si>
-    <t>olac:PrimaryText</t>
-  </si>
-  <si>
-    <t>PrimaryText</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#text</t>
-  </si>
-  <si>
-    <t>olac:Procedural</t>
-  </si>
-  <si>
-    <t>Procedural</t>
-  </si>
-  <si>
-    <t>olac:Report</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>olac:Singing</t>
-  </si>
-  <si>
     <t>Singing</t>
   </si>
   <si>
+    <t>olac:Speech</t>
+  </si>
+  <si>
+    <t>This resource contains a recording of one or more people speaking (NOT IN OLAC BUT NEEDED)</t>
+  </si>
+  <si>
+    <t>Speech</t>
+  </si>
+  <si>
     <t>olac:Syntactic</t>
   </si>
   <si>
+    <t>The resource contains annotation or other analysis describing  the syntactic structure of a PrimaryText</t>
+  </si>
+  <si>
     <t>Syntactic</t>
   </si>
   <si>
     <t>olac:Thesaurus</t>
   </si>
   <si>
+    <t xml:space="preserve">The resource contains  a list or data structure consisting  of words or concepts arranged according to sense.  
+</t>
+  </si>
+  <si>
     <t>Thesaurus</t>
   </si>
   <si>
@@ -277,6 +321,9 @@
     <t>olac:Transcription</t>
   </si>
   <si>
+    <t>The resource contains a written or coded annotation or analysis into another representation</t>
+  </si>
+  <si>
     <t>Transcription</t>
   </si>
   <si>
@@ -289,10 +336,22 @@
     <t>Translation</t>
   </si>
   <si>
-    <t>olac:Typed</t>
-  </si>
-  <si>
-    <t>Typed</t>
+    <t>olac:Typeset</t>
+  </si>
+  <si>
+    <t>The resource has been formatted for display</t>
+  </si>
+  <si>
+    <t>Typeset</t>
+  </si>
+  <si>
+    <t>olac:Typewritten</t>
+  </si>
+  <si>
+    <t>The resource was captured on a typewriter or a keyboard</t>
+  </si>
+  <si>
+    <t>Typewritten</t>
   </si>
   <si>
     <t>hasDefinedTerm</t>
@@ -304,19 +363,19 @@
     <t>DefinedTermSet</t>
   </si>
   <si>
-    <t>["olac:Thesaurus", "olac:Dialogue", "olac:Oratory", "olac:Report", "olac:Ludic", "olac:Procedural", "olac:Narrative", "olac:Interview", "olac:PartOfSpeech"]</t>
+    <t>["olac:Thesaurus", "olac:Dialogue", "olac:Oratory", "olac:Report", "olac:Ludic", "olac:Procedural", "olac:Narrative", "olac:Interview"]</t>
   </si>
   <si>
     <t>olac:CommunicationModeValues</t>
   </si>
   <si>
-    <t>["olac:Speech", "olac:Orthography", "olac:Singing", "olac:Code", "olac:Code", "HandWrtitten", "olac:NonDigitalWork", "olac:DigitalWork"]</t>
+    <t>["olac:Speech", "olac:Orthography", "olac:Singing", "olac:Code", "olac:Handwritten", "olac:Typewritten", "olac:Typeset", "olac:NotBornDigital", "olac:BornDigital"]</t>
   </si>
   <si>
     <t>olac:DerivedTextTypeValues</t>
   </si>
   <si>
-    <t>["olac:Phonemic", "olac:Phonetic", "olac:Phonological", "olac:Syntactic", "olac:Translation", "olac:Semantic", "Semantic", "olac:Transcription", "olac:Annotation"]</t>
+    <t>["olac:Phonemic", "olac:Phonetic", "olac:Phonological", "olac:Syntactic", "olac:Translation", "olac:Semantic", "olac:Transcription", "olac:Annotation"]</t>
   </si>
   <si>
     <t>olac:ResourceTypeValues</t>
@@ -325,33 +384,51 @@
     <t>["olac:PrimaryText", "olac:DerivedText"]</t>
   </si>
   <si>
+    <t>definedTermSet</t>
+  </si>
+  <si>
     <t>domainIncludes</t>
   </si>
   <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>rdfs:subPropertyOf</t>
+  </si>
+  <si>
     <t>rangeIncludes</t>
   </si>
   <si>
     <t>rdfs:comment</t>
   </si>
   <si>
-    <t>rdfs:label</t>
-  </si>
-  <si>
-    <t>definedTermSet</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
+    <t>olac:annotationType</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>"olac:DerivedTextTypeValues"</t>
+  </si>
+  <si>
+    <t>Annotation Type</t>
+  </si>
+  <si>
+    <t>annotationType</t>
+  </si>
+  <si>
     <t>olac:annotator</t>
   </si>
   <si>
-    <t>rdf:Property</t>
-  </si>
-  <si>
     <t>Annotator</t>
   </si>
   <si>
+    <t>annotator</t>
+  </si>
+  <si>
     <t>[, ]</t>
   </si>
   <si>
@@ -361,205 +438,247 @@
     <t>The participant produced an annotation of this or a related resource.</t>
   </si>
   <si>
-    <t>annotator</t>
-  </si>
-  <si>
     <t>olac:author</t>
   </si>
   <si>
     <t>Author</t>
   </si>
   <si>
+    <t>author</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#author</t>
   </si>
   <si>
     <t>The participant contributed original writings to the resource.</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>olac:communicationMode</t>
-  </si>
-  <si>
-    <t>communicationMode</t>
+    <t>olac:channels</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>Number of audio channels this resource contains (eg 1, 2 5.1)</t>
+  </si>
+  <si>
+    <t>olac:compiler</t>
+  </si>
+  <si>
+    <t>Compiler</t>
+  </si>
+  <si>
+    <t>compiler</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#compiler</t>
+  </si>
+  <si>
+    <t>The participant is responsible for collecting the sub-parts of the resource together.</t>
+  </si>
+  <si>
+    <t>This refers to someone who creates a single resource with multiple parts, such as a book of short stories, or a person who produces a corpus of resources, which may be archived separately.</t>
+  </si>
+  <si>
+    <t>A compiler of a book of short stories or a CD with several songs on it; a collector of a corpus of recordings in some language or on a given topic; a person who assembles a suite of software tools.</t>
+  </si>
+  <si>
+    <t>olac:consultant</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>consultant</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#consultant</t>
+  </si>
+  <si>
+    <t>The participant contributes expertise to the creation of a work.</t>
+  </si>
+  <si>
+    <t>This term is commonly used by field linguists for the native speakers who work with them in describing and analyzing a language. They contribute their expertise in their native language to the resource, although their speech, sign, or writing may not appear directly in the resource. In some parts of the world the preferred term for this role is "informant".</t>
+  </si>
+  <si>
+    <t>olac:dataInputter</t>
+  </si>
+  <si>
+    <t>Data Inputter</t>
+  </si>
+  <si>
+    <t>dataInputter</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#data_inputter</t>
+  </si>
+  <si>
+    <t>The participant was responsible for entering, re-typing, and/or structuring the data contained in the resource.</t>
+  </si>
+  <si>
+    <t>olac:depositor</t>
+  </si>
+  <si>
+    <t>Depositor</t>
+  </si>
+  <si>
+    <t>depositor</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#depositor</t>
+  </si>
+  <si>
+    <t>The participant was responsible for depositing the resource in an archive.</t>
+  </si>
+  <si>
+    <t>olac:developer</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#developer</t>
+  </si>
+  <si>
+    <t>The participant developed the methodology or tools that constitute the resource, or that were used to create the resource.</t>
+  </si>
+  <si>
+    <t>A software programmer, designer, or analyst; a designer of a questionnaire or research task.</t>
+  </si>
+  <si>
+    <t>olac:doi</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>A digital Object Identifier</t>
+  </si>
+  <si>
+    <t>olac:editor</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#editor</t>
+  </si>
+  <si>
+    <t>The participant reviewed, corrected, and/or tested the resource.</t>
+  </si>
+  <si>
+    <t>This role includes anyone whose role was editorial in nature, such as proof-readers, debuggers, testers, etc. It may overlap the Compiler role in some cases.</t>
+  </si>
+  <si>
+    <t>olac:hasAnnotation</t>
+  </si>
+  <si>
+    <t>Has Annotation</t>
+  </si>
+  <si>
+    <t>hasAnnotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This resource references another resource that describes it  such as a translation, transcription or other analysis </t>
+  </si>
+  <si>
+    <t>olac:illustrator</t>
+  </si>
+  <si>
+    <t>Illustrator</t>
+  </si>
+  <si>
+    <t>illustrator</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#illustrator</t>
+  </si>
+  <si>
+    <t>The participant contributed drawings or other illustrations to the resource.</t>
+  </si>
+  <si>
+    <t>olac:interpreter</t>
+  </si>
+  <si>
+    <t>Interpreter</t>
+  </si>
+  <si>
+    <t>interpreter</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#interpreter</t>
+  </si>
+  <si>
+    <t>The participant translates in real-time or explains the discourse recorded in the resource.</t>
+  </si>
+  <si>
+    <t>The choice between 'interpreter' and 'translator' may depend on the dynamics of the resource creation event or process. Generally, if the participant is translating 'live'; that is, while the speaker or signer is speaking or signing, she or he should be identified as an interpreter. Also, some discourse genres include a participant who interprets or explains a performance of some kind.</t>
+  </si>
+  <si>
+    <t>A person translating from English to ASL during a speech; a Kuna chief who interprets a chant that another chief has just performed, thus completing the ceremony.</t>
+  </si>
+  <si>
+    <t>olac:interviewer</t>
+  </si>
+  <si>
+    <t>Interviewer</t>
+  </si>
+  <si>
+    <t>interviewer</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#interviewer</t>
+  </si>
+  <si>
+    <t>The participant conducted an interview that forms part of the resource.</t>
+  </si>
+  <si>
+    <t>olac:isAnnotationOf</t>
+  </si>
+  <si>
+    <t>Is Annotation Of</t>
+  </si>
+  <si>
+    <t>isAnnotationOf</t>
+  </si>
+  <si>
+    <t>This resource contains some kind a description such as a translation, transcription or other analysis of the resource it references</t>
+  </si>
+  <si>
+    <t>olac:linguisticGenre</t>
+  </si>
+  <si>
+    <t>"olac:CommunicationGenreValues"</t>
+  </si>
+  <si>
+    <t>Linguistic Genre</t>
+  </si>
+  <si>
+    <t>linguisticGenre</t>
+  </si>
+  <si>
+    <t>olac:modality</t>
   </si>
   <si>
     <t>"olac:CommunicationModeValues"</t>
   </si>
   <si>
-    <t>olac:compiler</t>
-  </si>
-  <si>
-    <t>Compiler</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#compiler</t>
-  </si>
-  <si>
-    <t>The participant is responsible for collecting the sub-parts of the resource together.</t>
-  </si>
-  <si>
-    <t>compiler</t>
-  </si>
-  <si>
-    <t>This refers to someone who creates a single resource with multiple parts, such as a book of short stories, or a person who produces a corpus of resources, which may be archived separately.</t>
-  </si>
-  <si>
-    <t>A compiler of a book of short stories or a CD with several songs on it; a collector of a corpus of recordings in some language or on a given topic; a person who assembles a suite of software tools.</t>
-  </si>
-  <si>
-    <t>olac:connmunicationGenre</t>
-  </si>
-  <si>
-    <t>connmunicationGenre</t>
-  </si>
-  <si>
-    <t>"olac:CommunicationGenreValues"</t>
-  </si>
-  <si>
-    <t>olac:consultant</t>
-  </si>
-  <si>
-    <t>Consultant</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#consultant</t>
-  </si>
-  <si>
-    <t>The participant contributes expertise to the creation of a work.</t>
-  </si>
-  <si>
-    <t>consultant</t>
-  </si>
-  <si>
-    <t>This term is commonly used by field linguists for the native speakers who work with them in describing and analyzing a language. They contribute their expertise in their native language to the resource, although their speech, sign, or writing may not appear directly in the resource. In some parts of the world the preferred term for this role is "informant".</t>
-  </si>
-  <si>
-    <t>olac:data_inputter</t>
-  </si>
-  <si>
-    <t>Data Inputter</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#data_inputter</t>
-  </si>
-  <si>
-    <t>The participant was responsible for entering, re-typing, and/or structuring the data contained in the resource.</t>
-  </si>
-  <si>
-    <t>dataInputter</t>
-  </si>
-  <si>
-    <t>olac:depositor</t>
-  </si>
-  <si>
-    <t>Depositor</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#depositor</t>
-  </si>
-  <si>
-    <t>The participant was responsible for depositing the resource in an archive.</t>
-  </si>
-  <si>
-    <t>depositor</t>
-  </si>
-  <si>
-    <t>olac:derivedTextType</t>
-  </si>
-  <si>
-    <t>derivedTextType</t>
-  </si>
-  <si>
-    <t>"olac:DerivedTextTypeValues"</t>
-  </si>
-  <si>
-    <t>olac:developer</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#developer</t>
-  </si>
-  <si>
-    <t>The participant developed the methodology or tools that constitute the resource, or that were used to create the resource.</t>
-  </si>
-  <si>
-    <t>developer</t>
-  </si>
-  <si>
-    <t>A software programmer, designer, or analyst; a designer of a questionnaire or research task.</t>
-  </si>
-  <si>
-    <t>olac:editor</t>
-  </si>
-  <si>
-    <t>Editor</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#editor</t>
-  </si>
-  <si>
-    <t>The participant reviewed, corrected, and/or tested the resource.</t>
-  </si>
-  <si>
-    <t>editor</t>
-  </si>
-  <si>
-    <t>This role includes anyone whose role was editorial in nature, such as proof-readers, debuggers, testers, etc. It may overlap the Compiler role in some cases.</t>
-  </si>
-  <si>
-    <t>olac:illustrator</t>
-  </si>
-  <si>
-    <t>Illustrator</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#illustrator</t>
-  </si>
-  <si>
-    <t>The participant contributed drawings or other illustrations to the resource.</t>
-  </si>
-  <si>
-    <t>illustrator</t>
-  </si>
-  <si>
-    <t>olac:interpreter</t>
-  </si>
-  <si>
-    <t>Interpreter</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#interpreter</t>
-  </si>
-  <si>
-    <t>The participant translates in real-time or explains the discourse recorded in the resource.</t>
-  </si>
-  <si>
-    <t>interpreter</t>
-  </si>
-  <si>
-    <t>The choice between 'interpreter' and 'translator' may depend on the dynamics of the resource creation event or process. Generally, if the participant is translating 'live'; that is, while the speaker or signer is speaking or signing, she or he should be identified as an interpreter. Also, some discourse genres include a participant who interprets or explains a performance of some kind.</t>
-  </si>
-  <si>
-    <t>A person translating from English to ASL during a speech; a Kuna chief who interprets a chant that another chief has just performed, thus completing the ceremony.</t>
-  </si>
-  <si>
-    <t>olac:interviewer</t>
-  </si>
-  <si>
-    <t>Interviewer</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/role.html#interviewer</t>
-  </si>
-  <si>
-    <t>The participant conducted an interview that forms part of the resource.</t>
-  </si>
-  <si>
-    <t>interviewer</t>
+    <t>Modality</t>
+  </si>
+  <si>
+    <t>modality</t>
   </si>
   <si>
     <t>olac:participant</t>
@@ -568,15 +687,15 @@
     <t>Participant</t>
   </si>
   <si>
+    <t>participant</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#participant</t>
   </si>
   <si>
     <t>The participant was present during the creation of the resource, but did not contribute substantially to its content.</t>
   </si>
   <si>
-    <t>participant</t>
-  </si>
-  <si>
     <t>This role is intended for minor participants such as audience members or other peripherally-involved participants in the event. These interlocutors need not have been physically present. They could be participants in some form of long-distance communication, such as lurkers in an online discussion, or they may have participated in general sense of having allowed the creation event to take place, such as the mayor of an indigenous community.</t>
   </si>
   <si>
@@ -586,15 +705,15 @@
     <t>Performer</t>
   </si>
   <si>
+    <t>performer</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#performer</t>
   </si>
   <si>
     <t>The participant performed some portion of a recorded, filmed, or transcribed resource.</t>
   </si>
   <si>
-    <t>performer</t>
-  </si>
-  <si>
     <t>It is recommended that this term be used only for creative participants whose role is not better indicated by a more specific term, such as 'speaker', 'signer', or 'singer'.</t>
   </si>
   <si>
@@ -607,46 +726,49 @@
     <t>Person</t>
   </si>
   <si>
-    <t>This property references a Person item which represents the persistent identity of one or more ContributingPerson items</t>
-  </si>
-  <si>
     <t>person</t>
   </si>
   <si>
+    <t>This property references a Person item which represents the persistent identity of one or more ContributingPerson items.</t>
+  </si>
+  <si>
     <t>olac:photographer</t>
   </si>
   <si>
     <t>Photographer</t>
   </si>
   <si>
+    <t>photographer</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#photographer</t>
   </si>
   <si>
     <t>The participant took the photograph, or shot the film, that appears in or constitutes the resource.</t>
   </si>
   <si>
-    <t>photographer</t>
-  </si>
-  <si>
     <t>olac:recorder</t>
   </si>
   <si>
     <t>Recorder</t>
   </si>
   <si>
+    <t>recorder</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#recorder</t>
   </si>
   <si>
     <t>The participant operated the recording machinery used to create the resource.</t>
   </si>
   <si>
-    <t>recorder</t>
-  </si>
-  <si>
     <t>olac:register</t>
   </si>
   <si>
     <t>Register</t>
+  </si>
+  <si>
+    <t>register</t>
   </si>
   <si>
     <t>http://w3id.org/meta-share/meta-share/register</t>
@@ -656,54 +778,51 @@
 </t>
   </si>
   <si>
-    <t>register</t>
-  </si>
-  <si>
-    <t>olac:research_participant</t>
+    <t>olac:researchParticipant</t>
   </si>
   <si>
     <t>Research Participant</t>
   </si>
   <si>
+    <t>researchParticipant</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#research_participant</t>
   </si>
   <si>
     <t>The participant acted as a research subject or responded to a questionnaire, the results of which study form the basis of the resource.</t>
   </si>
   <si>
-    <t>researchParticipant</t>
-  </si>
-  <si>
     <t>olac:researcher</t>
   </si>
   <si>
     <t>Researcher</t>
   </si>
   <si>
+    <t>researcher</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#researcher</t>
   </si>
   <si>
     <t>The resource was created as part of the participant's research, or the research presents interim or final results from the participant's research.</t>
   </si>
   <si>
-    <t>researcher</t>
-  </si>
-  <si>
     <t>olac:responder</t>
   </si>
   <si>
     <t>Responder</t>
   </si>
   <si>
+    <t>responder</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#responder</t>
   </si>
   <si>
     <t>The participant was an interlocutor in some sort of discourse event.</t>
   </si>
   <si>
-    <t>responder</t>
-  </si>
-  <si>
     <t>This person's voice can be heard (or their words can be read) in the resource, typically saying the language-appropriate equivalent of "uh-huh", "amen", "you don't say", etc. This role is sometimes referred to as a "yes-sayer", "backchanneler, or "co-conversant".</t>
   </si>
   <si>
@@ -713,15 +832,15 @@
     <t>Signer</t>
   </si>
   <si>
+    <t>signer</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#signer</t>
   </si>
   <si>
     <t>The participant was a principal signer in a resource that consists of a recording, a film, or a transcription of a recorded resource.</t>
   </si>
   <si>
-    <t>signer</t>
-  </si>
-  <si>
     <t>Signers are those whose gestures predominate in a recorded or filmed resource. (This resource may be a transcription of that recording.)</t>
   </si>
   <si>
@@ -734,30 +853,30 @@
     <t>Singer</t>
   </si>
   <si>
+    <t>singer</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#singer</t>
   </si>
   <si>
     <t>The participant sang, either individually or as part of a group, in a resource that consists of a recording, a film, or a transcription of a recorded resource.</t>
   </si>
   <si>
-    <t>singer</t>
-  </si>
-  <si>
     <t>olac:speaker</t>
   </si>
   <si>
     <t>Speaker</t>
   </si>
   <si>
+    <t>speaker</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#speaker</t>
   </si>
   <si>
     <t>The participant was a principal speaker in a resource that consists of a recording, a film, or a transcription of a recorded resource.</t>
   </si>
   <si>
-    <t>speaker</t>
-  </si>
-  <si>
     <t>Speakers are those whose voices predominate in a recorded or filmed resource. (This resource may be a transcription of that recording.)</t>
   </si>
   <si>
@@ -770,45 +889,45 @@
     <t>Sponsor</t>
   </si>
   <si>
+    <t>sponsor</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#sponsor</t>
   </si>
   <si>
     <t>The participant contributed financial support to the creation of the resource.</t>
   </si>
   <si>
-    <t>sponsor</t>
-  </si>
-  <si>
     <t>olac:transcriber</t>
   </si>
   <si>
     <t>Transcriber</t>
   </si>
   <si>
+    <t>transcriber</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#transcriber</t>
   </si>
   <si>
     <t>The participant produced a transcription of this or a related resource.</t>
   </si>
   <si>
-    <t>transcriber</t>
-  </si>
-  <si>
     <t>olac:translator</t>
   </si>
   <si>
     <t>Translator</t>
   </si>
   <si>
+    <t>translator</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#translator</t>
   </si>
   <si>
     <t>The participant produced a translation of this or a related resource.</t>
   </si>
   <si>
-    <t>translator</t>
-  </si>
-  <si>
     <t>rdfs:subClassOf</t>
   </si>
   <si>
@@ -821,7 +940,7 @@
     <t xml:space="preserve">This class represents a snapshot of a Person in time, in their role as a contributor to one or more creative works. The purpose of this class  is to caputre the metadata that applies to a person at a particular time, as their name, age, gender, social status  etc may be different over time. </t>
   </si>
   <si>
-    <t>ContributingPerson</t>
+    <t>PersonSnapshot</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1467,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -1362,29 +1481,35 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1393,16 +1518,13 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,29 +1532,29 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1441,9 +1563,9 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
       <c r="E6" t="s">
@@ -1455,27 +1577,30 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,313 +1608,397 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>75</v>
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
       </c>
       <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +2023,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -1822,41 +2031,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -1864,16 +2073,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1884,13 +2093,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L34"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="11" width="20" customWidth="1"/>
+    <col min="1" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1898,731 +2107,790 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>103</v>
-      </c>
       <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" t="s">
-        <v>106</v>
-      </c>
       <c r="J1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>140</v>
+      </c>
+      <c r="F4" t="s">
+        <v>141</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="J5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>149</v>
+      </c>
+      <c r="F6" t="s">
+        <v>150</v>
       </c>
       <c r="H6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="I6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="J6" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" t="s">
         <v>136</v>
       </c>
-      <c r="H7" t="s">
-        <v>137</v>
+      <c r="I7" t="s">
+        <v>158</v>
       </c>
       <c r="J7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="K7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="H8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>146</v>
-      </c>
-      <c r="G9" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="H9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I9" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>172</v>
+      </c>
+      <c r="F10" t="s">
+        <v>173</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>174</v>
+      </c>
+      <c r="J10" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G11" t="s">
-        <v>155</v>
-      </c>
-      <c r="H11" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="J11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G12" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="I12" t="s">
+        <v>184</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="K12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="F13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" t="s">
-        <v>167</v>
-      </c>
-      <c r="H13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="J13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="F14" t="s">
-        <v>171</v>
-      </c>
-      <c r="G14" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>173</v>
+        <v>136</v>
+      </c>
+      <c r="I14" t="s">
+        <v>194</v>
       </c>
       <c r="J14" t="s">
-        <v>174</v>
-      </c>
-      <c r="K14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>197</v>
       </c>
       <c r="F15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G15" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="H15" t="s">
-        <v>180</v>
+        <v>136</v>
+      </c>
+      <c r="I15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J15" t="s">
+        <v>200</v>
+      </c>
+      <c r="K15" t="s">
+        <v>201</v>
+      </c>
+      <c r="L15" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>204</v>
       </c>
       <c r="F16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G16" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="H16" t="s">
-        <v>185</v>
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>206</v>
       </c>
       <c r="J16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" t="s">
-        <v>188</v>
+        <v>129</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" t="s">
-        <v>190</v>
-      </c>
-      <c r="H17" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="J17" t="s">
-        <v>192</v>
-      </c>
-      <c r="K17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" t="s">
-        <v>195</v>
-      </c>
-      <c r="G18" t="s">
-        <v>196</v>
-      </c>
-      <c r="H18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="C18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" t="s">
-        <v>199</v>
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>217</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
-      </c>
-      <c r="G19" t="s">
-        <v>201</v>
-      </c>
-      <c r="H19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" t="s">
-        <v>204</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
-      </c>
-      <c r="G20" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="H20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J20" t="s">
+        <v>224</v>
+      </c>
+      <c r="K20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" t="s">
-        <v>209</v>
+        <v>129</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>227</v>
       </c>
       <c r="F21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G21" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="H21" t="s">
-        <v>212</v>
+        <v>136</v>
+      </c>
+      <c r="I21" t="s">
+        <v>229</v>
       </c>
       <c r="J21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="K21" t="s">
+        <v>231</v>
+      </c>
+      <c r="L21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" t="s">
-        <v>214</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G22" t="s">
-        <v>216</v>
-      </c>
-      <c r="H22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="J22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>220</v>
-      </c>
-      <c r="G23" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="H23" t="s">
-        <v>222</v>
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
+        <v>240</v>
+      </c>
+      <c r="J23" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" t="s">
-        <v>224</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="F24" t="s">
-        <v>225</v>
-      </c>
-      <c r="G24" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="H24" t="s">
-        <v>227</v>
+        <v>136</v>
+      </c>
+      <c r="I24" t="s">
+        <v>245</v>
       </c>
       <c r="J24" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>230</v>
+        <v>129</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="F25" t="s">
-        <v>231</v>
-      </c>
-      <c r="G25" t="s">
-        <v>232</v>
-      </c>
-      <c r="H25" t="s">
-        <v>233</v>
+        <v>249</v>
+      </c>
+      <c r="I25" t="s">
+        <v>250</v>
       </c>
       <c r="J25" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="K25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" t="s">
-        <v>237</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>253</v>
       </c>
       <c r="F26" t="s">
-        <v>238</v>
-      </c>
-      <c r="G26" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="H26" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I26" t="s">
+        <v>255</v>
+      </c>
+      <c r="J26" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" t="s">
-        <v>242</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>258</v>
       </c>
       <c r="F27" t="s">
-        <v>243</v>
-      </c>
-      <c r="G27" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="H27" t="s">
-        <v>245</v>
+        <v>136</v>
+      </c>
+      <c r="I27" t="s">
+        <v>260</v>
       </c>
       <c r="J27" t="s">
-        <v>246</v>
-      </c>
-      <c r="K27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" t="s">
-        <v>249</v>
+        <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="F28" t="s">
-        <v>250</v>
-      </c>
-      <c r="G28" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="H28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I28" t="s">
+        <v>265</v>
+      </c>
+      <c r="J28" t="s">
+        <v>266</v>
+      </c>
+      <c r="K28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" t="s">
-        <v>254</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>269</v>
       </c>
       <c r="F29" t="s">
-        <v>255</v>
-      </c>
-      <c r="G29" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="H29" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I29" t="s">
+        <v>271</v>
+      </c>
+      <c r="J29" t="s">
+        <v>272</v>
+      </c>
+      <c r="K29" t="s">
+        <v>273</v>
+      </c>
+      <c r="L29" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" t="s">
-        <v>259</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>276</v>
       </c>
       <c r="F30" t="s">
-        <v>260</v>
-      </c>
-      <c r="G30" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="H30" t="s">
-        <v>262</v>
+        <v>136</v>
+      </c>
+      <c r="I30" t="s">
+        <v>278</v>
+      </c>
+      <c r="J30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>280</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" t="s">
+        <v>281</v>
+      </c>
+      <c r="F31" t="s">
+        <v>282</v>
+      </c>
+      <c r="H31" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" t="s">
+        <v>283</v>
+      </c>
+      <c r="J31" t="s">
+        <v>284</v>
+      </c>
+      <c r="K31" t="s">
+        <v>285</v>
+      </c>
+      <c r="L31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>287</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" t="s">
+        <v>288</v>
+      </c>
+      <c r="F32" t="s">
+        <v>289</v>
+      </c>
+      <c r="H32" t="s">
+        <v>136</v>
+      </c>
+      <c r="I32" t="s">
+        <v>290</v>
+      </c>
+      <c r="J32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F33" t="s">
+        <v>294</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" t="s">
+        <v>295</v>
+      </c>
+      <c r="J33" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" t="s">
+        <v>298</v>
+      </c>
+      <c r="F34" t="s">
+        <v>299</v>
+      </c>
+      <c r="H34" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" t="s">
+        <v>300</v>
+      </c>
+      <c r="J34" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2650,13 +2918,13 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2664,19 +2932,19 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>305</v>
       </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved layout of markdown file, added licenses and fixed bug with values going missing in spreadsheet
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -9,15 +9,15 @@
     <sheet sheetId="3" name="@type=Thing" state="visible" r:id="rId6"/>
     <sheet sheetId="4" name="@type=DefinedTerm" state="visible" r:id="rId7"/>
     <sheet sheetId="5" name="@type=DefinedTermSet" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="@type=rdfProperty" state="visible" r:id="rId9"/>
-    <sheet sheetId="7" name="@type=rdfsClass" state="visible" r:id="rId10"/>
+    <sheet sheetId="6" name="@type=rdfsClass" state="visible" r:id="rId9"/>
+    <sheet sheetId="7" name="@type=rdfProperty" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="291">
   <si>
     <t>Name</t>
   </si>
@@ -384,18 +384,72 @@
     <t>["olac:PrimaryText", "olac:DerivedText"]</t>
   </si>
   <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>rdfs:subClassOf</t>
+  </si>
+  <si>
+    <t>olac:OrganizationBasedLicense</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>OrganizationBasedLicense</t>
+  </si>
+  <si>
+    <t>A licence document  setting out rights and oblications could be based copyright or other rights  based on membership of an Organization. The organization could be any  group of people with appropriate governance from self selected individuals who agree to license terms, to groups of researchers, to ad-hoc groups of members of a community</t>
+  </si>
+  <si>
+    <t>{"@id":"schema:CreativeWork"}</t>
+  </si>
+  <si>
+    <t>olac:OrganizationDepositLicense</t>
+  </si>
+  <si>
+    <t>OrganizationDepositLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A license document setting out terms for deposit into a repository by one or more identified groups </t>
+  </si>
+  <si>
+    <t>"olac:OrganizationBasedLicense"</t>
+  </si>
+  <si>
+    <t>olac:OrganizationReuseLicense</t>
+  </si>
+  <si>
+    <t>OrganizationReuseLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A license document setting out terms for reuse of data by one or more identified groups </t>
+  </si>
+  <si>
+    <t>olac:PersonSnapshot</t>
+  </si>
+  <si>
+    <t>PersonSnapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class represents a snapshot of a Person in time, in their role as a contributor to one or more creative works. The purpose of this class  is to caputre the metadata that applies to a person at a particular time, as their name, age, gender, social status  etc may be different over time. </t>
+  </si>
+  <si>
+    <t>[{"@id":"schema:Person"}, {"@id":"schema:Role"}]</t>
+  </si>
+  <si>
     <t>definedTermSet</t>
   </si>
   <si>
-    <t>rdfs:label</t>
+    <t>domainIncludes</t>
   </si>
   <si>
     <t>rangeIncludes</t>
   </si>
   <si>
-    <t>rdfs:comment</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
@@ -408,21 +462,18 @@
     <t>"olac:DerivedTextTypeValues"</t>
   </si>
   <si>
-    <t>Annotation Type</t>
-  </si>
-  <si>
     <t>annotationType</t>
   </si>
   <si>
     <t>olac:annotator</t>
   </si>
   <si>
-    <t>Annotator</t>
-  </si>
-  <si>
     <t>annotator</t>
   </si>
   <si>
+    <t>[{"@id":"schema:Person"}, {"@id":"schema:Organization"}]</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/role.html#annotator</t>
   </si>
   <si>
@@ -432,9 +483,6 @@
     <t>olac:author</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
@@ -447,9 +495,6 @@
     <t>olac:channels</t>
   </si>
   <si>
-    <t>Channels</t>
-  </si>
-  <si>
     <t>channels</t>
   </si>
   <si>
@@ -459,9 +504,6 @@
     <t>olac:compiler</t>
   </si>
   <si>
-    <t>Compiler</t>
-  </si>
-  <si>
     <t>compiler</t>
   </si>
   <si>
@@ -480,9 +522,6 @@
     <t>olac:consultant</t>
   </si>
   <si>
-    <t>Consultant</t>
-  </si>
-  <si>
     <t>consultant</t>
   </si>
   <si>
@@ -498,9 +537,6 @@
     <t>olac:dataInputter</t>
   </si>
   <si>
-    <t>Data Inputter</t>
-  </si>
-  <si>
     <t>dataInputter</t>
   </si>
   <si>
@@ -513,9 +549,6 @@
     <t>olac:depositor</t>
   </si>
   <si>
-    <t>Depositor</t>
-  </si>
-  <si>
     <t>depositor</t>
   </si>
   <si>
@@ -528,9 +561,6 @@
     <t>olac:developer</t>
   </si>
   <si>
-    <t>Developer</t>
-  </si>
-  <si>
     <t>developer</t>
   </si>
   <si>
@@ -546,9 +576,6 @@
     <t>olac:doi</t>
   </si>
   <si>
-    <t>DOI</t>
-  </si>
-  <si>
     <t>doi</t>
   </si>
   <si>
@@ -558,9 +585,6 @@
     <t>olac:editor</t>
   </si>
   <si>
-    <t>Editor</t>
-  </si>
-  <si>
     <t>editor</t>
   </si>
   <si>
@@ -576,9 +600,6 @@
     <t>olac:hasAnnotation</t>
   </si>
   <si>
-    <t>Has Annotation</t>
-  </si>
-  <si>
     <t>hasAnnotation</t>
   </si>
   <si>
@@ -588,9 +609,6 @@
     <t>olac:illustrator</t>
   </si>
   <si>
-    <t>Illustrator</t>
-  </si>
-  <si>
     <t>illustrator</t>
   </si>
   <si>
@@ -603,9 +621,6 @@
     <t>olac:interpreter</t>
   </si>
   <si>
-    <t>Interpreter</t>
-  </si>
-  <si>
     <t>interpreter</t>
   </si>
   <si>
@@ -624,9 +639,6 @@
     <t>olac:interviewer</t>
   </si>
   <si>
-    <t>Interviewer</t>
-  </si>
-  <si>
     <t>interviewer</t>
   </si>
   <si>
@@ -639,24 +651,33 @@
     <t>olac:isAnnotationOf</t>
   </si>
   <si>
-    <t>Is Annotation Of</t>
-  </si>
-  <si>
     <t>isAnnotationOf</t>
   </si>
   <si>
     <t>This resource contains some kind a description such as a translation, transcription or other analysis of the resource it references</t>
   </si>
   <si>
+    <t>olac:licensedOrganization</t>
+  </si>
+  <si>
+    <t>licensedOrganization</t>
+  </si>
+  <si>
+    <t>{"@id":"schema:Orgnization"}</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/role.html#translator</t>
+  </si>
+  <si>
+    <t>Indicates a group of people who have the rights described in this license</t>
+  </si>
+  <si>
     <t>olac:linguisticGenre</t>
   </si>
   <si>
     <t>"olac:CommunicationGenreValues"</t>
   </si>
   <si>
-    <t>Linguistic Genre</t>
-  </si>
-  <si>
     <t>linguisticGenre</t>
   </si>
   <si>
@@ -666,18 +687,12 @@
     <t>"olac:CommunicationModeValues"</t>
   </si>
   <si>
-    <t>Modality</t>
-  </si>
-  <si>
     <t>modality</t>
   </si>
   <si>
     <t>olac:participant</t>
   </si>
   <si>
-    <t>Participant</t>
-  </si>
-  <si>
     <t>participant</t>
   </si>
   <si>
@@ -693,9 +708,6 @@
     <t>olac:performer</t>
   </si>
   <si>
-    <t>Performer</t>
-  </si>
-  <si>
     <t>performer</t>
   </si>
   <si>
@@ -714,21 +726,21 @@
     <t>olac:person</t>
   </si>
   <si>
-    <t>Person</t>
+    <t>"olac:PersonSnapshot"</t>
   </si>
   <si>
     <t>person</t>
   </si>
   <si>
+    <t>{"@id":"schema:Person"}</t>
+  </si>
+  <si>
     <t>This property references a Person item which represents the persistent identity of one or more ContributingPerson items.</t>
   </si>
   <si>
     <t>olac:photographer</t>
   </si>
   <si>
-    <t>Photographer</t>
-  </si>
-  <si>
     <t>photographer</t>
   </si>
   <si>
@@ -741,9 +753,6 @@
     <t>olac:recorder</t>
   </si>
   <si>
-    <t>Recorder</t>
-  </si>
-  <si>
     <t>recorder</t>
   </si>
   <si>
@@ -754,9 +763,6 @@
   </si>
   <si>
     <t>olac:register</t>
-  </si>
-  <si>
-    <t>Register</t>
   </si>
   <si>
     <t>register</t>
@@ -772,9 +778,6 @@
     <t>olac:researchParticipant</t>
   </si>
   <si>
-    <t>Research Participant</t>
-  </si>
-  <si>
     <t>researchParticipant</t>
   </si>
   <si>
@@ -787,9 +790,6 @@
     <t>olac:researcher</t>
   </si>
   <si>
-    <t>Researcher</t>
-  </si>
-  <si>
     <t>researcher</t>
   </si>
   <si>
@@ -802,9 +802,6 @@
     <t>olac:responder</t>
   </si>
   <si>
-    <t>Responder</t>
-  </si>
-  <si>
     <t>responder</t>
   </si>
   <si>
@@ -820,9 +817,6 @@
     <t>olac:signer</t>
   </si>
   <si>
-    <t>Signer</t>
-  </si>
-  <si>
     <t>signer</t>
   </si>
   <si>
@@ -841,9 +835,6 @@
     <t>olac:singer</t>
   </si>
   <si>
-    <t>Singer</t>
-  </si>
-  <si>
     <t>singer</t>
   </si>
   <si>
@@ -856,9 +847,6 @@
     <t>olac:speaker</t>
   </si>
   <si>
-    <t>Speaker</t>
-  </si>
-  <si>
     <t>speaker</t>
   </si>
   <si>
@@ -877,9 +865,6 @@
     <t>olac:sponsor</t>
   </si>
   <si>
-    <t>Sponsor</t>
-  </si>
-  <si>
     <t>sponsor</t>
   </si>
   <si>
@@ -892,9 +877,6 @@
     <t>olac:transcriber</t>
   </si>
   <si>
-    <t>Transcriber</t>
-  </si>
-  <si>
     <t>transcriber</t>
   </si>
   <si>
@@ -907,31 +889,10 @@
     <t>olac:translator</t>
   </si>
   <si>
-    <t>Translator</t>
-  </si>
-  <si>
     <t>translator</t>
   </si>
   <si>
-    <t>http://www.language-archives.org/REC/role.html#translator</t>
-  </si>
-  <si>
     <t>The participant produced a translation of this or a related resource.</t>
-  </si>
-  <si>
-    <t>rdfs:subClassOf</t>
-  </si>
-  <si>
-    <t>rdfs:Class</t>
-  </si>
-  <si>
-    <t>Analytical Lexicon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This class represents a snapshot of a Person in time, in their role as a contributor to one or more creative works. The purpose of this class  is to caputre the metadata that applies to a person at a particular time, as their name, age, gender, social status  etc may be different over time. </t>
-  </si>
-  <si>
-    <t>PersonSnapshot</t>
   </si>
 </sst>
 </file>
@@ -2084,13 +2045,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2098,10 +2059,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>122</v>
@@ -2109,773 +2070,85 @@
       <c r="F1" t="s">
         <v>123</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>124</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="B2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
         <v>132</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>133</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
         <v>134</v>
       </c>
-      <c r="H3" t="s">
+      <c r="D4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>136</v>
       </c>
-      <c r="B4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
         <v>137</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
         <v>138</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
         <v>139</v>
-      </c>
-      <c r="H4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" t="s">
-        <v>149</v>
-      </c>
-      <c r="I6" t="s">
-        <v>150</v>
-      </c>
-      <c r="J6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>155</v>
-      </c>
-      <c r="H7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E9" t="s">
-        <v>165</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12" t="s">
-        <v>182</v>
-      </c>
-      <c r="I12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" t="s">
-        <v>186</v>
-      </c>
-      <c r="H13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" t="s">
-        <v>190</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
-        <v>191</v>
-      </c>
-      <c r="H14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" t="s">
-        <v>194</v>
-      </c>
-      <c r="E15" t="s">
-        <v>195</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" t="s">
-        <v>196</v>
-      </c>
-      <c r="H15" t="s">
-        <v>197</v>
-      </c>
-      <c r="I15" t="s">
-        <v>198</v>
-      </c>
-      <c r="J15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E16" t="s">
-        <v>202</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" t="s">
-        <v>203</v>
-      </c>
-      <c r="H16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" t="s">
-        <v>207</v>
-      </c>
-      <c r="H17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" t="s">
-        <v>210</v>
-      </c>
-      <c r="D18" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>213</v>
-      </c>
-      <c r="B19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D19" t="s">
-        <v>215</v>
-      </c>
-      <c r="E19" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>217</v>
-      </c>
-      <c r="B20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" t="s">
-        <v>218</v>
-      </c>
-      <c r="E20" t="s">
-        <v>219</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>220</v>
-      </c>
-      <c r="H20" t="s">
-        <v>221</v>
-      </c>
-      <c r="I20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>223</v>
-      </c>
-      <c r="B21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" t="s">
-        <v>224</v>
-      </c>
-      <c r="E21" t="s">
-        <v>225</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" t="s">
-        <v>226</v>
-      </c>
-      <c r="H21" t="s">
-        <v>227</v>
-      </c>
-      <c r="I21" t="s">
-        <v>228</v>
-      </c>
-      <c r="J21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" t="s">
-        <v>231</v>
-      </c>
-      <c r="E22" t="s">
-        <v>232</v>
-      </c>
-      <c r="H22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>234</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>235</v>
-      </c>
-      <c r="E23" t="s">
-        <v>236</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" t="s">
-        <v>237</v>
-      </c>
-      <c r="H23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" t="s">
-        <v>240</v>
-      </c>
-      <c r="E24" t="s">
-        <v>241</v>
-      </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" t="s">
-        <v>242</v>
-      </c>
-      <c r="H24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" t="s">
-        <v>245</v>
-      </c>
-      <c r="E25" t="s">
-        <v>246</v>
-      </c>
-      <c r="G25" t="s">
-        <v>247</v>
-      </c>
-      <c r="H25" t="s">
-        <v>248</v>
-      </c>
-      <c r="I25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" t="s">
-        <v>250</v>
-      </c>
-      <c r="E26" t="s">
-        <v>251</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>252</v>
-      </c>
-      <c r="H26" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>254</v>
-      </c>
-      <c r="B27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" t="s">
-        <v>255</v>
-      </c>
-      <c r="E27" t="s">
-        <v>256</v>
-      </c>
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" t="s">
-        <v>257</v>
-      </c>
-      <c r="H27" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>259</v>
-      </c>
-      <c r="B28" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" t="s">
-        <v>260</v>
-      </c>
-      <c r="E28" t="s">
-        <v>261</v>
-      </c>
-      <c r="F28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" t="s">
-        <v>262</v>
-      </c>
-      <c r="H28" t="s">
-        <v>263</v>
-      </c>
-      <c r="I28" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>265</v>
-      </c>
-      <c r="B29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" t="s">
-        <v>266</v>
-      </c>
-      <c r="E29" t="s">
-        <v>267</v>
-      </c>
-      <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" t="s">
-        <v>268</v>
-      </c>
-      <c r="H29" t="s">
-        <v>269</v>
-      </c>
-      <c r="I29" t="s">
-        <v>270</v>
-      </c>
-      <c r="J29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>272</v>
-      </c>
-      <c r="B30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" t="s">
-        <v>273</v>
-      </c>
-      <c r="E30" t="s">
-        <v>274</v>
-      </c>
-      <c r="F30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" t="s">
-        <v>275</v>
-      </c>
-      <c r="H30" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>277</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" t="s">
-        <v>278</v>
-      </c>
-      <c r="E31" t="s">
-        <v>279</v>
-      </c>
-      <c r="F31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" t="s">
-        <v>280</v>
-      </c>
-      <c r="H31" t="s">
-        <v>281</v>
-      </c>
-      <c r="I31" t="s">
-        <v>282</v>
-      </c>
-      <c r="J31" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>284</v>
-      </c>
-      <c r="B32" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" t="s">
-        <v>285</v>
-      </c>
-      <c r="E32" t="s">
-        <v>286</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" t="s">
-        <v>287</v>
-      </c>
-      <c r="H32" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>289</v>
-      </c>
-      <c r="B33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" t="s">
-        <v>291</v>
-      </c>
-      <c r="F33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" t="s">
-        <v>292</v>
-      </c>
-      <c r="H33" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>294</v>
-      </c>
-      <c r="B34" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" t="s">
-        <v>295</v>
-      </c>
-      <c r="E34" t="s">
-        <v>296</v>
-      </c>
-      <c r="F34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" t="s">
-        <v>297</v>
-      </c>
-      <c r="H34" t="s">
-        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2886,13 +2159,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K35"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2900,36 +2173,915 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" t="s">
-        <v>299</v>
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>302</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>303</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" t="s">
+        <v>182</v>
+      </c>
+      <c r="J10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" t="s">
+        <v>197</v>
+      </c>
+      <c r="I14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" t="s">
+        <v>201</v>
+      </c>
+      <c r="I15" t="s">
+        <v>202</v>
+      </c>
+      <c r="J15" t="s">
+        <v>203</v>
+      </c>
+      <c r="K15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" t="s">
+        <v>210</v>
+      </c>
+      <c r="I17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G18" t="s">
+        <v>214</v>
+      </c>
+      <c r="H18" t="s">
+        <v>215</v>
+      </c>
+      <c r="I18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" t="s">
+        <v>219</v>
+      </c>
+      <c r="F19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" t="s">
+        <v>224</v>
+      </c>
+      <c r="G21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" t="s">
+        <v>225</v>
+      </c>
+      <c r="I21" t="s">
+        <v>226</v>
+      </c>
+      <c r="J21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" t="s">
+        <v>229</v>
+      </c>
+      <c r="G22" t="s">
+        <v>150</v>
+      </c>
+      <c r="H22" t="s">
+        <v>230</v>
+      </c>
+      <c r="I22" t="s">
+        <v>231</v>
+      </c>
+      <c r="J22" t="s">
+        <v>232</v>
+      </c>
+      <c r="K22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" t="s">
+        <v>236</v>
+      </c>
+      <c r="G23" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F24" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" t="s">
+        <v>241</v>
+      </c>
+      <c r="I24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
+        <v>244</v>
+      </c>
+      <c r="F25" t="s">
+        <v>244</v>
+      </c>
+      <c r="G25" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" t="s">
+        <v>245</v>
+      </c>
+      <c r="I25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>247</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" t="s">
+        <v>248</v>
+      </c>
+      <c r="F26" t="s">
+        <v>248</v>
+      </c>
+      <c r="H26" t="s">
+        <v>249</v>
+      </c>
+      <c r="I26" t="s">
+        <v>250</v>
+      </c>
+      <c r="J26" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>251</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" t="s">
+        <v>252</v>
+      </c>
+      <c r="F27" t="s">
+        <v>252</v>
+      </c>
+      <c r="G27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" t="s">
+        <v>253</v>
+      </c>
+      <c r="I27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>256</v>
+      </c>
+      <c r="F28" t="s">
+        <v>256</v>
+      </c>
+      <c r="G28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" t="s">
+        <v>257</v>
+      </c>
+      <c r="I28" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" t="s">
+        <v>260</v>
+      </c>
+      <c r="F29" t="s">
+        <v>260</v>
+      </c>
+      <c r="G29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" t="s">
+        <v>261</v>
+      </c>
+      <c r="I29" t="s">
+        <v>262</v>
+      </c>
+      <c r="J29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" t="s">
+        <v>265</v>
+      </c>
+      <c r="F30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G30" t="s">
+        <v>150</v>
+      </c>
+      <c r="H30" t="s">
+        <v>266</v>
+      </c>
+      <c r="I30" t="s">
+        <v>267</v>
+      </c>
+      <c r="J30" t="s">
+        <v>268</v>
+      </c>
+      <c r="K30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" t="s">
+        <v>271</v>
+      </c>
+      <c r="G31" t="s">
+        <v>150</v>
+      </c>
+      <c r="H31" t="s">
+        <v>272</v>
+      </c>
+      <c r="I31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" t="s">
+        <v>275</v>
+      </c>
+      <c r="F32" t="s">
+        <v>275</v>
+      </c>
+      <c r="G32" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" t="s">
+        <v>276</v>
+      </c>
+      <c r="I32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J32" t="s">
+        <v>278</v>
+      </c>
+      <c r="K32" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" t="s">
+        <v>281</v>
+      </c>
+      <c r="F33" t="s">
+        <v>281</v>
+      </c>
+      <c r="G33" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" t="s">
+        <v>282</v>
+      </c>
+      <c r="I33" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>284</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F34" t="s">
+        <v>285</v>
+      </c>
+      <c r="G34" t="s">
+        <v>150</v>
+      </c>
+      <c r="H34" t="s">
+        <v>286</v>
+      </c>
+      <c r="I34" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>288</v>
+      </c>
+      <c r="B35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" t="s">
+        <v>289</v>
+      </c>
+      <c r="F35" t="s">
+        <v>289</v>
+      </c>
+      <c r="G35" t="s">
+        <v>150</v>
+      </c>
+      <c r="H35" t="s">
+        <v>215</v>
+      </c>
+      <c r="I35" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further tidyups, added a couple of classes to make it eaiser to have Properties
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -7,9 +7,9 @@
     <sheet sheetId="1" name="RootDataset" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="@context" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="@type=Thing" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="@type=DefinedTerm" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="@type=DefinedTermSet" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="@type=rdfsClass" state="visible" r:id="rId9"/>
+    <sheet sheetId="4" name="@type=rdfsClass" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="@type=DefinedTerm" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="@type=DefinedTermSet" state="visible" r:id="rId9"/>
     <sheet sheetId="7" name="@type=rdfProperty" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="312">
   <si>
     <t>Name</t>
   </si>
@@ -82,49 +82,112 @@
     <t>sameAs</t>
   </si>
   <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>rdfs:subClassOf</t>
+  </si>
+  <si>
+    <t>#a4f96dd6-dcc5-4d98-8bef-775a5d946650</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>PrimaryText</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text</t>
+  </si>
+  <si>
+    <t>This is a primary resource: the object of study.   A text is defined as any primary resource or research material, such as a literary work, film, or recording of natural discourse</t>
+  </si>
+  <si>
+    <t>{"@id":"schema:CreativeWork"}</t>
+  </si>
+  <si>
     <t>olac:Annotation</t>
   </si>
   <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#annotation</t>
+  </si>
+  <si>
+    <t>The resource includes information which annotates, describes or otherwise an some other linguistic record.</t>
+  </si>
+  <si>
+    <t>olac:DerivedText</t>
+  </si>
+  <si>
+    <t>DerivedText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A resource is derived from another resource, via some automated process, eg a downsampled video or an abstract of a text which  is not an analytical product </t>
+  </si>
+  <si>
+    <t>olac:OrganizationBasedLicense</t>
+  </si>
+  <si>
+    <t>OrganizationBasedLicense</t>
+  </si>
+  <si>
+    <t>A licence document  setting out rights and oblications could be based copyright or other rights  based on membership of an Organization. The organization could be any  group of people with appropriate governance from self selected individuals who agree to license terms, to groups of researchers, to ad-hoc groups of members of a community</t>
+  </si>
+  <si>
+    <t>olac:OrganizationDepositLicense</t>
+  </si>
+  <si>
+    <t>OrganizationDepositLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A license document setting out terms for deposit into a repository by one or more identified groups </t>
+  </si>
+  <si>
+    <t>"olac:OrganizationBasedLicense"</t>
+  </si>
+  <si>
+    <t>olac:OrganizationReuseLicense</t>
+  </si>
+  <si>
+    <t>OrganizationReuseLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A license document setting out terms for reuse of data by one or more identified groups </t>
+  </si>
+  <si>
+    <t>olac:PersonSnapshot</t>
+  </si>
+  <si>
+    <t>PersonSnapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class represents a snapshot of a Person in time, in their role as a contributor to one or more creative works. The purpose of this class  is to caputre the metadata that applies to a person at a particular time, as their name, age, gender, social status  etc may be different over time. </t>
+  </si>
+  <si>
+    <t>[{"@id":"schema:Person"}, {"@id":"schema:Role"}]</t>
+  </si>
+  <si>
+    <t>olac:PrimaryText</t>
+  </si>
+  <si>
+    <t>olac:Code</t>
+  </si>
+  <si>
     <t>DefinedTerm</t>
   </si>
   <si>
-    <t>The resource includes information which annotates, describes or otherwise an some other linguistic record.</t>
-  </si>
-  <si>
-    <t>Annotation</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#annotation</t>
-  </si>
-  <si>
-    <t>olac:BornDigital</t>
+    <t>The resource contains a coded analysis or annotation</t>
   </si>
   <si>
     <t>CommunicationModeValues</t>
   </si>
   <si>
-    <t>BornDigital</t>
-  </si>
-  <si>
-    <t>olac:Code</t>
-  </si>
-  <si>
-    <t>The resource contains a coded analysis or annotation</t>
-  </si>
-  <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t>olac:DerivedText</t>
-  </si>
-  <si>
-    <t>The resource is derivied from another resource, eg a downsampled video or an abstract of a text but is not an analytical product</t>
-  </si>
-  <si>
-    <t>ResourceTypeValues</t>
-  </si>
-  <si>
-    <t>DerivedText</t>
   </si>
   <si>
     <t>olac:Dialogue</t>
@@ -206,21 +269,6 @@
     <t>Narrative</t>
   </si>
   <si>
-    <t>olac:NonDigital</t>
-  </si>
-  <si>
-    <t>The resource was not originally captured or created  in digital form</t>
-  </si>
-  <si>
-    <t>NonDigital</t>
-  </si>
-  <si>
-    <t>olac:NotBornDigital</t>
-  </si>
-  <si>
-    <t>NotBornDigital</t>
-  </si>
-  <si>
     <t>olac:Oratory</t>
   </si>
   <si>
@@ -260,18 +308,6 @@
     <t>Phonological</t>
   </si>
   <si>
-    <t>olac:PrimaryText</t>
-  </si>
-  <si>
-    <t>This is a primary resource: the object of study.   A text is defined as any primary resource or research material, such as a literary work, film, or recording of natural discourse</t>
-  </si>
-  <si>
-    <t>PrimaryText</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#text</t>
-  </si>
-  <si>
     <t>olac:Procedural</t>
   </si>
   <si>
@@ -290,6 +326,15 @@
     <t>Report</t>
   </si>
   <si>
+    <t>olac:Semantic</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Speech</t>
+  </si>
+  <si>
     <t>olac:Singing</t>
   </si>
   <si>
@@ -303,9 +348,6 @@
   </si>
   <si>
     <t>This resource contains a recording of one or more people speaking (NOT IN OLAC BUT NEEDED)</t>
-  </si>
-  <si>
-    <t>Speech</t>
   </si>
   <si>
     <t>olac:Syntactic</t>
@@ -330,6 +372,18 @@
     <t>http://www.language-archives.org/REC/type-20020628.html#text/singing</t>
   </si>
   <si>
+    <t>olac:TimeAligned</t>
+  </si>
+  <si>
+    <t>The resource contains a written or coded annotation(s) which has data aligning the annotation(s)  with a PrimaryText</t>
+  </si>
+  <si>
+    <t>TimeAligned</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#transcription</t>
+  </si>
+  <si>
     <t>olac:Transcription</t>
   </si>
   <si>
@@ -339,9 +393,6 @@
     <t>Transcription</t>
   </si>
   <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#transcription</t>
-  </si>
-  <si>
     <t>olac:Translation</t>
   </si>
   <si>
@@ -354,13 +405,16 @@
     <t>The resource has been formatted for display</t>
   </si>
   <si>
+    <t>"olac:OrthographyTypeValues"</t>
+  </si>
+  <si>
     <t>Typeset</t>
   </si>
   <si>
     <t>olac:Typewritten</t>
   </si>
   <si>
-    <t>The resource was captured on a typewriter or a keyboard</t>
+    <t>The annotation has time-alignement with the PrimaryText</t>
   </si>
   <si>
     <t>Typewritten</t>
@@ -375,19 +429,28 @@
     <t>DefinedTermSet</t>
   </si>
   <si>
-    <t>["olac:Thesaurus", "olac:Dialogue", "olac:Oratory", "olac:Report", "olac:Ludic", "olac:Procedural", "olac:Narrative", "olac:Interview", , "olac:Informational"]]</t>
+    <t>["olac:Thesaurus", "olac:Dialogue", "olac:Oratory", "olac:Report", "olac:Ludic", "olac:Procedural", "olac:Narrative", "olac:Interview", "olac:Drama", "olac:Informational"]</t>
   </si>
   <si>
     <t>olac:CommunicationModeValues</t>
   </si>
   <si>
-    <t>["olac:Speech", "olac:Orthography", "olac:Singing", "olac:Code", "olac:Handwritten", "olac:Typewritten", "olac:Typeset", "olac:NotBornDigital", "olac:BornDigital"]</t>
+    <t>["olac:Speech", "olac:Orthography", "olac:Singing", "olac:Gesture"]</t>
   </si>
   <si>
     <t>olac:DerivedTextTypeValues</t>
   </si>
   <si>
-    <t>["olac:Phonemic", "olac:Phonetic", "olac:Phonological", "olac:Syntactic", "olac:Translation", "olac:Semantic", "olac:Transcription", "olac:Annotation"]</t>
+    <t>["olac:Phonemic", "olac:Phonetic", "olac:Phonological", "olac:Syntactic", "olac:Translation", "olac:Semantic", "olac:Transcription", "olac:TimeAligned", "olac:Prosodic"]</t>
+  </si>
+  <si>
+    <t>AnnotationTypeValues</t>
+  </si>
+  <si>
+    <t>olac:OrthographyTypeValues</t>
+  </si>
+  <si>
+    <t>["olac:Handwritten", "olac:Typewritten", "olac:Typeset"]</t>
   </si>
   <si>
     <t>olac:ResourceTypeValues</t>
@@ -396,61 +459,7 @@
     <t>["olac:PrimaryText", "olac:DerivedText", "olac:Annotation"]</t>
   </si>
   <si>
-    <t>rdfs:comment</t>
-  </si>
-  <si>
-    <t>rdfs:label</t>
-  </si>
-  <si>
-    <t>rdfs:subClassOf</t>
-  </si>
-  <si>
-    <t>olac:OrganizationBasedLicense</t>
-  </si>
-  <si>
-    <t>rdfs:Class</t>
-  </si>
-  <si>
-    <t>OrganizationBasedLicense</t>
-  </si>
-  <si>
-    <t>A licence document  setting out rights and oblications could be based copyright or other rights  based on membership of an Organization. The organization could be any  group of people with appropriate governance from self selected individuals who agree to license terms, to groups of researchers, to ad-hoc groups of members of a community</t>
-  </si>
-  <si>
-    <t>{"@id":"schema:CreativeWork"}</t>
-  </si>
-  <si>
-    <t>olac:OrganizationDepositLicense</t>
-  </si>
-  <si>
-    <t>OrganizationDepositLicense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A license document setting out terms for deposit into a repository by one or more identified groups </t>
-  </si>
-  <si>
-    <t>"olac:OrganizationBasedLicense"</t>
-  </si>
-  <si>
-    <t>olac:OrganizationReuseLicense</t>
-  </si>
-  <si>
-    <t>OrganizationReuseLicense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A license document setting out terms for reuse of data by one or more identified groups </t>
-  </si>
-  <si>
-    <t>olac:PersonSnapshot</t>
-  </si>
-  <si>
-    <t>PersonSnapshot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This class represents a snapshot of a Person in time, in their role as a contributor to one or more creative works. The purpose of this class  is to caputre the metadata that applies to a person at a particular time, as their name, age, gender, social status  etc may be different over time. </t>
-  </si>
-  <si>
-    <t>[{"@id":"schema:Person"}, {"@id":"schema:Role"}]</t>
+    <t>ResourceTypeValues</t>
   </si>
   <si>
     <t>definedTermSet</t>
@@ -474,6 +483,9 @@
     <t>"olac:DerivedTextTypeValues"</t>
   </si>
   <si>
+    <t>"olac:Annotation"</t>
+  </si>
+  <si>
     <t>annotationType</t>
   </si>
   <si>
@@ -609,9 +621,27 @@
     <t>This role includes anyone whose role was editorial in nature, such as proof-readers, debuggers, testers, etc. It may overlap the Compiler role in some cases.</t>
   </si>
   <si>
+    <t>olac:geoJSON</t>
+  </si>
+  <si>
+    <t>[{"@id":"schema:GeoCoordinates"}, {"@id":"schema:GeoShape"}, {"@id":"schema:Language"}]</t>
+  </si>
+  <si>
+    <t>geoJSON</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A valid GEOJson feature or feature collection as a string that can be parsed as JSON </t>
+  </si>
+  <si>
     <t>olac:hasAnnotation</t>
   </si>
   <si>
+    <t>"olac:PrimaryText"</t>
+  </si>
+  <si>
     <t>hasAnnotation</t>
   </si>
   <si>
@@ -675,7 +705,7 @@
     <t>licensedOrganization</t>
   </si>
   <si>
-    <t>{"@id":"schema:Orgnization"}</t>
+    <t>{"@id":"schema:Organization"}</t>
   </si>
   <si>
     <t>http://www.language-archives.org/REC/role.html#translator</t>
@@ -687,10 +717,10 @@
     <t>olac:linguisticGenre</t>
   </si>
   <si>
-    <t>"olac:CommunicationGenreValues"</t>
-  </si>
-  <si>
-    <t>linguisticGenre</t>
+    <t>orthographyType</t>
+  </si>
+  <si>
+    <t>NOTE: This is required for Nyingarn – do we want to have a further set of types for SungText, SpokenText, GesturedText, OrthographicText so that they can each have special sub-type properties</t>
   </si>
   <si>
     <t>olac:modality</t>
@@ -836,6 +866,15 @@
   </si>
   <si>
     <t>This person's voice can be heard (or their words can be read) in the resource, typically saying the language-appropriate equivalent of "uh-huh", "amen", "you don't say", etc. This role is sometimes referred to as a "yes-sayer", "backchanneler, or "co-conversant".</t>
+  </si>
+  <si>
+    <t>olac:scriptType</t>
+  </si>
+  <si>
+    <t>"olac:CommunicationGenreValues"</t>
+  </si>
+  <si>
+    <t>scriptType</t>
   </si>
   <si>
     <t>olac:signer</t>
@@ -1443,7 +1482,216 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G9"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -1469,532 +1717,467 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
+      <c r="D12" t="s">
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
       </c>
       <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>37</v>
-      </c>
       <c r="E26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>123</v>
+      </c>
+      <c r="F27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2003,9 +2186,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="20" customWidth="1"/>
@@ -2019,7 +2202,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2027,172 +2210,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" t="s">
         <v>135</v>
       </c>
-      <c r="E3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" t="s">
-        <v>143</v>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2286,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K38"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2217,938 +2300,984 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" t="s">
-        <v>158</v>
-      </c>
-      <c r="G4" t="s">
-        <v>154</v>
-      </c>
       <c r="H4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="I6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I7" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="J7" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F8" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F9" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H10" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="I11" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G12" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I12" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J12" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>202</v>
+      </c>
+      <c r="G13" t="s">
+        <v>203</v>
       </c>
       <c r="I13" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="F14" t="s">
-        <v>200</v>
-      </c>
-      <c r="G14" t="s">
-        <v>154</v>
-      </c>
-      <c r="H14" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="I14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="G15" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="I15" t="s">
-        <v>206</v>
-      </c>
-      <c r="J15" t="s">
-        <v>207</v>
-      </c>
-      <c r="K15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G16" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I16" t="s">
-        <v>212</v>
+        <v>216</v>
+      </c>
+      <c r="J16" t="s">
+        <v>217</v>
+      </c>
+      <c r="K16" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="F17" t="s">
-        <v>214</v>
+        <v>220</v>
+      </c>
+      <c r="G17" t="s">
+        <v>158</v>
+      </c>
+      <c r="H17" t="s">
+        <v>221</v>
       </c>
       <c r="I17" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="F18" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G18" t="s">
-        <v>218</v>
-      </c>
-      <c r="H18" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="I18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="G19" t="s">
+        <v>228</v>
+      </c>
+      <c r="H19" t="s">
+        <v>229</v>
+      </c>
+      <c r="I19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="F20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="C21" t="s">
+        <v>235</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G21" t="s">
-        <v>154</v>
-      </c>
-      <c r="H21" t="s">
-        <v>229</v>
-      </c>
-      <c r="I21" t="s">
-        <v>230</v>
-      </c>
-      <c r="J21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F22" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="G22" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H22" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I22" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="J22" t="s">
-        <v>236</v>
-      </c>
-      <c r="K22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>239</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F23" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G23" t="s">
-        <v>241</v>
+        <v>158</v>
+      </c>
+      <c r="H23" t="s">
+        <v>244</v>
       </c>
       <c r="I23" t="s">
-        <v>242</v>
+        <v>245</v>
+      </c>
+      <c r="J23" t="s">
+        <v>246</v>
+      </c>
+      <c r="K23" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
       <c r="E24" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="F24" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
-      </c>
-      <c r="H24" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="I24" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="F25" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H25" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="I25" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F26" t="s">
-        <v>252</v>
+        <v>258</v>
+      </c>
+      <c r="G26" t="s">
+        <v>158</v>
       </c>
       <c r="H26" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="I26" t="s">
-        <v>254</v>
-      </c>
-      <c r="J26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="F27" t="s">
-        <v>256</v>
-      </c>
-      <c r="G27" t="s">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="H27" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="I27" t="s">
-        <v>258</v>
+        <v>264</v>
+      </c>
+      <c r="J27" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F28" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H28" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I28" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" t="s">
-        <v>264</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="F29" t="s">
-        <v>265</v>
+        <v>270</v>
+      </c>
+      <c r="G29" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" t="s">
+        <v>271</v>
       </c>
       <c r="I29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="C30" t="s">
+        <v>274</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="F30" t="s">
-        <v>268</v>
-      </c>
-      <c r="G30" t="s">
-        <v>154</v>
-      </c>
-      <c r="H30" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I30" t="s">
-        <v>270</v>
-      </c>
-      <c r="J30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="F31" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="G31" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H31" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="I31" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="J31" t="s">
-        <v>276</v>
-      </c>
-      <c r="K31" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" t="s">
-        <v>132</v>
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>283</v>
       </c>
       <c r="E32" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F32" t="s">
-        <v>279</v>
-      </c>
-      <c r="G32" t="s">
-        <v>154</v>
-      </c>
-      <c r="H32" t="s">
-        <v>280</v>
-      </c>
-      <c r="I32" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F33" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G33" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H33" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="I33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="J33" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="K33" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B34" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F34" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H34" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="I34" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F35" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G35" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H35" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="I35" t="s">
-        <v>295</v>
+        <v>298</v>
+      </c>
+      <c r="J35" t="s">
+        <v>299</v>
+      </c>
+      <c r="K35" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F36" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="G36" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>219</v>
+        <v>303</v>
       </c>
       <c r="I36" t="s">
-        <v>298</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>305</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>306</v>
+      </c>
+      <c r="F37" t="s">
+        <v>306</v>
+      </c>
+      <c r="G37" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" t="s">
+        <v>307</v>
+      </c>
+      <c r="I37" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
+        <v>310</v>
+      </c>
+      <c r="F38" t="s">
+        <v>310</v>
+      </c>
+      <c r="G38" t="s">
+        <v>158</v>
+      </c>
+      <c r="H38" t="s">
+        <v>229</v>
+      </c>
+      <c r="I38" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tool to look add vocab terms (not language  specific so needs to move somewhere)
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="311">
   <si>
     <t>Name</t>
   </si>
@@ -700,6 +700,21 @@
   </si>
   <si>
     <t>This resource contains some kind a description such as a translation, transcription or other analysis of the resource it references</t>
+  </si>
+  <si>
+    <t>olac:isDeIdentified</t>
+  </si>
+  <si>
+    <t>[{"@id":"schema:CreativeWork"}, {"@id":"schema:Person"}, olac:PersonSnapshot]</t>
+  </si>
+  <si>
+    <t>isDeIdentified</t>
+  </si>
+  <si>
+    <t>{"@id":"schema:Boolean"}</t>
+  </si>
+  <si>
+    <t>This data in this item has had identifying information removed, or in the case of a person the name is an alias</t>
   </si>
   <si>
     <t>olac:licensedOrganization</t>
@@ -2245,7 +2260,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2730,94 +2745,88 @@
         <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="E19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G19" t="s">
-        <v>229</v>
-      </c>
-      <c r="H19" t="s">
         <v>230</v>
       </c>
       <c r="I19" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>232</v>
       </c>
       <c r="B20" t="s">
         <v>152</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
         <v>233</v>
       </c>
-      <c r="D20" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>233</v>
+      </c>
+      <c r="G20" t="s">
         <v>234</v>
       </c>
-      <c r="F20" t="s">
-        <v>234</v>
+      <c r="H20" t="s">
+        <v>235</v>
+      </c>
+      <c r="I20" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s">
         <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>206</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
         <v>152</v>
+      </c>
+      <c r="C22" t="s">
+        <v>241</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F22" t="s">
-        <v>239</v>
-      </c>
-      <c r="G22" t="s">
-        <v>158</v>
-      </c>
-      <c r="H22" t="s">
-        <v>240</v>
-      </c>
-      <c r="I22" t="s">
-        <v>241</v>
-      </c>
-      <c r="J22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>243</v>
       </c>
@@ -2845,30 +2854,36 @@
       <c r="J23" t="s">
         <v>247</v>
       </c>
-      <c r="K23" t="s">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
         <v>249</v>
       </c>
-      <c r="B24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
+        <v>249</v>
+      </c>
+      <c r="G24" t="s">
+        <v>158</v>
+      </c>
+      <c r="H24" t="s">
         <v>250</v>
       </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
         <v>251</v>
       </c>
-      <c r="F24" t="s">
-        <v>251</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="J24" t="s">
         <v>252</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2880,27 +2895,24 @@
         <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>255</v>
       </c>
       <c r="E25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G25" t="s">
-        <v>158</v>
-      </c>
-      <c r="H25" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B26" t="s">
         <v>152</v>
@@ -2909,24 +2921,24 @@
         <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G26" t="s">
         <v>158</v>
       </c>
       <c r="H26" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I26" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B27" t="s">
         <v>152</v>
@@ -2935,24 +2947,24 @@
         <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F27" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="G27" t="s">
+        <v>158</v>
       </c>
       <c r="H27" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I27" t="s">
-        <v>265</v>
-      </c>
-      <c r="J27" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B28" t="s">
         <v>152</v>
@@ -2961,24 +2973,24 @@
         <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F28" t="s">
-        <v>267</v>
-      </c>
-      <c r="G28" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="H28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I28" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="J28" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B29" t="s">
         <v>152</v>
@@ -2987,24 +2999,24 @@
         <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F29" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G29" t="s">
         <v>158</v>
       </c>
       <c r="H29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I29" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B30" t="s">
         <v>152</v>
@@ -3013,25 +3025,22 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
       </c>
       <c r="H30" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I30" t="s">
-        <v>277</v>
-      </c>
-      <c r="J30" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>279</v>
       </c>
@@ -3059,13 +3068,10 @@
       <c r="J31" t="s">
         <v>283</v>
       </c>
-      <c r="K31" t="s">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>285</v>
       </c>
       <c r="B32" t="s">
         <v>152</v>
@@ -3074,24 +3080,30 @@
         <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G32" t="s">
         <v>158</v>
       </c>
       <c r="H32" t="s">
+        <v>286</v>
+      </c>
+      <c r="I32" t="s">
         <v>287</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B33" t="s">
         <v>152</v>
@@ -3100,30 +3112,24 @@
         <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F33" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G33" t="s">
         <v>158</v>
       </c>
       <c r="H33" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I33" t="s">
-        <v>292</v>
-      </c>
-      <c r="J33" t="s">
         <v>293</v>
       </c>
-      <c r="K33" t="s">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>295</v>
       </c>
       <c r="B34" t="s">
         <v>152</v>
@@ -3132,24 +3138,30 @@
         <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G34" t="s">
         <v>158</v>
       </c>
       <c r="H34" t="s">
+        <v>296</v>
+      </c>
+      <c r="I34" t="s">
         <v>297</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>298</v>
+      </c>
+      <c r="K34" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B35" t="s">
         <v>152</v>
@@ -3158,24 +3170,24 @@
         <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F35" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G35" t="s">
         <v>158</v>
       </c>
       <c r="H35" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I35" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B36" t="s">
         <v>152</v>
@@ -3184,19 +3196,45 @@
         <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F36" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G36" t="s">
         <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="I36" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>309</v>
+      </c>
+      <c r="F37" t="s">
+        <v>309</v>
+      </c>
+      <c r="G37" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" t="s">
+        <v>235</v>
+      </c>
+      <c r="I37" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new classes and associated props: CollectionProtocol and CollectionEvent
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="363">
   <si>
     <t>Name</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Thing</t>
   </si>
   <si>
-    <t>DerivedTextTypeValues</t>
+    <t>DerivedTextTypeTerms</t>
   </si>
   <si>
     <t>sameAs</t>
@@ -109,6 +109,27 @@
     <t>{"@id":"schema:CreativeWork"}</t>
   </si>
   <si>
+    <t>txc:CollectionEvent</t>
+  </si>
+  <si>
+    <t>CollectionEvent</t>
+  </si>
+  <si>
+    <t>A description of an event at which one or more PrimaryTexts were captured,  eg as video or audio</t>
+  </si>
+  <si>
+    <t>[{"@id":"schema:Event"}, {"@id":"schema:CreateAction"}]</t>
+  </si>
+  <si>
+    <t>txc:CollectionProtocol</t>
+  </si>
+  <si>
+    <t>CollectionProtocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of how this Object or Collection was obtained – such as strategy used for selecting orthographic text, or the prompts given to participants </t>
+  </si>
+  <si>
     <t>txc:DerivedText</t>
   </si>
   <si>
@@ -181,7 +202,7 @@
     <t>The resource contains a coded analysis or annotation</t>
   </si>
   <si>
-    <t>CommunicationModeValues</t>
+    <t>CommunicationModeTerms</t>
   </si>
   <si>
     <t>Code</t>
@@ -193,10 +214,36 @@
     <t>An interactive discourse with two or more participants. Examples of dialogues include conversations, interviews, correspondence, consultations, greetings and leave-takings.</t>
   </si>
   <si>
-    <t>CommunicationGenreValues</t>
+    <t>CommunicationGenreTerms</t>
   </si>
   <si>
     <t>Dialogue</t>
+  </si>
+  <si>
+    <t>txc:Drama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A planned, creative, rendition of discourse with two or more participants.
+</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/drama</t>
+  </si>
+  <si>
+    <t>txc:Formulaic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The resource is a ritually or conventionally structured discourse.
+</t>
+  </si>
+  <si>
+    <t>Formulaic</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/formulaic</t>
   </si>
   <si>
     <t>txc:Gesture</t>
@@ -335,6 +382,22 @@
     <t>Semantic</t>
   </si>
   <si>
+    <t>txc:Session</t>
+  </si>
+  <si>
+    <t>A collection event which is a recording or elicitation Session with particpants</t>
+  </si>
+  <si>
+    <t>"txc:OrthographyTypeTerms"</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mpi.nl/ISLE/documents/draft/ISLE_MetaData_2.5.pdf
+</t>
+  </si>
+  <si>
     <t>txc:Singing</t>
   </si>
   <si>
@@ -360,6 +423,18 @@
   </si>
   <si>
     <t>Syntactic</t>
+  </si>
+  <si>
+    <t>txc:Task</t>
+  </si>
+  <si>
+    <t>The collection protocol includes a task-based prompt to partipants</t>
+  </si>
+  <si>
+    <t>"txc:CollectionProtocolTypeTerms"</t>
+  </si>
+  <si>
+    <t>Task</t>
   </si>
   <si>
     <t>txc:Thesaurus</t>
@@ -408,9 +483,6 @@
     <t>The resource has been formatted for display</t>
   </si>
   <si>
-    <t>"txc:OrthographyTypeValues"</t>
-  </si>
-  <si>
     <t>Typeset</t>
   </si>
   <si>
@@ -426,19 +498,31 @@
     <t>hasDefinedTerm</t>
   </si>
   <si>
-    <t>txc:CommunicationGenreValues</t>
+    <t>txc:CollectionEventTypeTerms</t>
   </si>
   <si>
     <t>DefinedTermSet</t>
   </si>
   <si>
-    <t>["txc:Thesaurus", "txc:Dialogue", "txc:Oratory", "txc:Report", "txc:Ludic", "txc:Procedural", "txc:Narrative", "txc:Interview", "txc:Drama", "txc:Informational"]</t>
+    <t>"txc:Session"</t>
+  </si>
+  <si>
+    <t>txc:CollectionProtocolTypeTerms</t>
+  </si>
+  <si>
+    <t>"txc:Task"</t>
+  </si>
+  <si>
+    <t>txc:CommunicationGenreTerms</t>
+  </si>
+  <si>
+    <t>["txc:Thesaurus", "txc:Dialogue", "txc:Oratory", "txc:Report", "txc:Ludic", "txc:Procedural", "txc:Narrative", "txc:Interview", "txc:Drama", "txc:Informational", "txc:formulaic"]</t>
   </si>
   <si>
     <t>LinguistcGenreTerms</t>
   </si>
   <si>
-    <t>txc:CommunicationModeValues</t>
+    <t>txc:CommunicationModeTerms</t>
   </si>
   <si>
     <t>["txc:Speech", "txc:Orthography", "txc:Singing", "txc:Gesture"]</t>
@@ -447,7 +531,7 @@
     <t>ModalityTerms</t>
   </si>
   <si>
-    <t>txc:DerivedTextTypeValues</t>
+    <t>txc:DerivedTextTypeTerms</t>
   </si>
   <si>
     <t>["txc:Phonemic", "txc:Phonetic", "txc:Phonological", "txc:Syntactic", "txc:Translation", "txc:Semantic", "txc:Transcription", "txc:TimeAligned", "txc:Prosodic"]</t>
@@ -456,12 +540,15 @@
     <t>AnnotationTypeTerms</t>
   </si>
   <si>
-    <t>txc:OrthographyTypeValues</t>
+    <t>txc:OrthographyTypeTerms</t>
   </si>
   <si>
     <t>["txc:Handwritten", "txc:Typewritten", "txc:Typeset"]</t>
   </si>
   <si>
+    <t>OrthographyTypeTerms</t>
+  </si>
+  <si>
     <t>domainIncludes</t>
   </si>
   <si>
@@ -498,7 +585,7 @@
     <t>annotationType</t>
   </si>
   <si>
-    <t>"txc:DerivedTextTypeValues"</t>
+    <t>"txc:DerivedTextTypeTerms"</t>
   </si>
   <si>
     <t>txc:annotator</t>
@@ -537,6 +624,33 @@
     <t>Number of audio channels this resource contains (eg 1, 2 5.1)</t>
   </si>
   <si>
+    <t>txc:collectionEventType</t>
+  </si>
+  <si>
+    <t>"txc:CollectionEvent"</t>
+  </si>
+  <si>
+    <t>collectionEventType</t>
+  </si>
+  <si>
+    <t>An event with a start and end time during which data are gathered from partipants, or from other materials</t>
+  </si>
+  <si>
+    <t>"txc:CollectionEventTypeTerms"</t>
+  </si>
+  <si>
+    <t>txc:collectionProtocolType</t>
+  </si>
+  <si>
+    <t>"txc:CollectionProtocol"</t>
+  </si>
+  <si>
+    <t>collectionProtocolType</t>
+  </si>
+  <si>
+    <t>A description of the process used to collect or collate data, such as prompts given to participants, or how texts are selected for inclusion in a collection</t>
+  </si>
+  <si>
     <t>txc:compiler</t>
   </si>
   <si>
@@ -783,7 +897,7 @@
     <t>linguisticGenre</t>
   </si>
   <si>
-    <t>"txc:CommunicationGenreValues"</t>
+    <t>"txc:CommunicationGenreTerms"</t>
   </si>
   <si>
     <t>txc:modality</t>
@@ -792,7 +906,7 @@
     <t>modality</t>
   </si>
   <si>
-    <t>"txc:CommunicationModeValues"</t>
+    <t>"txc:CommunicationModeTerms"</t>
   </si>
   <si>
     <t>txc:participant</t>
@@ -1524,7 +1638,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="20" customWidth="1"/>
@@ -1586,17 +1700,14 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,14 +1740,17 @@
       <c r="C5" t="s">
         <v>38</v>
       </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1656,7 +1770,7 @@
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1689,9 +1803,6 @@
       <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
       <c r="E8" t="s">
         <v>50</v>
       </c>
@@ -1699,6 +1810,49 @@
         <v>49</v>
       </c>
       <c r="G8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1710,7 +1864,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F34"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -1738,468 +1892,545 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
+      <c r="C4" t="s">
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
       <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="F10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D27" t="s">
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
       </c>
       <c r="D28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
         <v>19</v>
       </c>
-      <c r="E28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>127</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" t="s">
-        <v>129</v>
-      </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>144</v>
+      </c>
+      <c r="F30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2210,7 +2441,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="20" customWidth="1"/>
@@ -2224,7 +2455,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -2232,58 +2463,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2294,7 +2553,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2308,13 +2567,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
@@ -2323,7 +2582,7 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
@@ -2332,1038 +2591,1084 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="H3" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F4" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="I5" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="F6" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E7" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="F7" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" t="s">
-        <v>175</v>
-      </c>
-      <c r="J7" t="s">
-        <v>176</v>
-      </c>
-      <c r="K7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="H7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="G8" t="s">
-        <v>179</v>
-      </c>
-      <c r="I8" t="s">
-        <v>181</v>
-      </c>
-      <c r="J8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="I9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="J9" t="s">
+        <v>213</v>
+      </c>
+      <c r="K9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="I10" t="s">
+        <v>218</v>
+      </c>
+      <c r="J10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E11" t="s">
-        <v>194</v>
-      </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="I11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="E12" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="G12" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="I12" t="s">
-        <v>199</v>
-      </c>
-      <c r="J12" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>229</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>230</v>
+      </c>
+      <c r="E13" t="s">
+        <v>231</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="G13" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F14" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="G14" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="I14" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="J14" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E15" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="F15" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="E16" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="F16" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="G16" t="s">
-        <v>215</v>
+        <v>242</v>
+      </c>
+      <c r="I16" t="s">
+        <v>244</v>
+      </c>
+      <c r="J16" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>247</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="G17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>253</v>
       </c>
       <c r="F18" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="G18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18" t="s">
-        <v>223</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="E19" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F19" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F20" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="G20" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="I20" t="s">
-        <v>231</v>
-      </c>
-      <c r="J20" t="s">
-        <v>232</v>
-      </c>
-      <c r="K20" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>263</v>
       </c>
       <c r="F21" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="G21" t="s">
-        <v>235</v>
-      </c>
-      <c r="I21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="E22" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F22" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="G22" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="I22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+      <c r="J22" t="s">
+        <v>269</v>
+      </c>
+      <c r="K22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>242</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="E23" t="s">
-        <v>244</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="G23" t="s">
-        <v>246</v>
+        <v>272</v>
+      </c>
+      <c r="I23" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="E24" t="s">
-        <v>249</v>
+        <v>190</v>
       </c>
       <c r="F24" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="G24" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="I24" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="D25" t="s">
-        <v>253</v>
+        <v>280</v>
+      </c>
+      <c r="E25" t="s">
+        <v>281</v>
+      </c>
+      <c r="F25" t="s">
+        <v>282</v>
       </c>
       <c r="G25" t="s">
-        <v>253</v>
-      </c>
-      <c r="H25" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>256</v>
+        <v>285</v>
+      </c>
+      <c r="E26" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26" t="s">
+        <v>287</v>
       </c>
       <c r="G26" t="s">
-        <v>256</v>
-      </c>
-      <c r="H26" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="I26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
       <c r="D27" t="s">
-        <v>259</v>
-      </c>
-      <c r="E27" t="s">
-        <v>162</v>
-      </c>
-      <c r="F27" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="G27" t="s">
-        <v>259</v>
-      </c>
-      <c r="I27" t="s">
-        <v>261</v>
-      </c>
-      <c r="J27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="H27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>264</v>
-      </c>
-      <c r="E28" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="G28" t="s">
-        <v>264</v>
-      </c>
-      <c r="I28" t="s">
-        <v>266</v>
-      </c>
-      <c r="J28" t="s">
-        <v>267</v>
-      </c>
-      <c r="K28" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="H28" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
       <c r="E29" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
       <c r="F29" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="G29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="I29" t="s">
+        <v>298</v>
+      </c>
+      <c r="J29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="E30" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F30" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="G30" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="I30" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="J30" t="s">
+        <v>304</v>
+      </c>
+      <c r="K30" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>307</v>
       </c>
       <c r="D31" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>309</v>
       </c>
       <c r="F31" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="G31" t="s">
-        <v>279</v>
-      </c>
-      <c r="I31" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>283</v>
+        <v>312</v>
+      </c>
+      <c r="E32" t="s">
+        <v>190</v>
       </c>
       <c r="F32" t="s">
-        <v>284</v>
+        <v>313</v>
       </c>
       <c r="G32" t="s">
-        <v>283</v>
+        <v>312</v>
       </c>
       <c r="I32" t="s">
-        <v>285</v>
-      </c>
-      <c r="J32" t="s">
-        <v>284</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>286</v>
+        <v>315</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F33" t="s">
-        <v>288</v>
+        <v>317</v>
       </c>
       <c r="G33" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="I33" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>290</v>
+        <v>319</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>291</v>
-      </c>
-      <c r="E34" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="F34" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="G34" t="s">
-        <v>291</v>
+        <v>320</v>
       </c>
       <c r="I34" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="J34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F35" t="s">
-        <v>296</v>
+        <v>325</v>
       </c>
       <c r="G35" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I35" t="s">
-        <v>297</v>
-      </c>
-      <c r="J35" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="E36" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F36" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="G36" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="I36" t="s">
-        <v>302</v>
-      </c>
-      <c r="J36" t="s">
-        <v>303</v>
-      </c>
-      <c r="K36" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>305</v>
+        <v>331</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="E37" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F37" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="G37" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="I37" t="s">
-        <v>308</v>
+        <v>334</v>
+      </c>
+      <c r="J37" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C38" t="s">
         <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F38" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="G38" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
       <c r="I38" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="J38" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="K38" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="E39" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F39" t="s">
-        <v>317</v>
+        <v>344</v>
       </c>
       <c r="G39" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="I39" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="G40" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="I40" t="s">
-        <v>322</v>
+        <v>349</v>
+      </c>
+      <c r="J40" t="s">
+        <v>350</v>
+      </c>
+      <c r="K40" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="E41" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F41" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="G41" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="I41" t="s">
-        <v>251</v>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>356</v>
+      </c>
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s">
+        <v>357</v>
+      </c>
+      <c r="E42" t="s">
+        <v>190</v>
+      </c>
+      <c r="F42" t="s">
+        <v>358</v>
+      </c>
+      <c r="G42" t="s">
+        <v>357</v>
+      </c>
+      <c r="I42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>360</v>
+      </c>
+      <c r="B43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>361</v>
+      </c>
+      <c r="E43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" t="s">
+        <v>362</v>
+      </c>
+      <c r="G43" t="s">
+        <v>361</v>
+      </c>
+      <c r="I43" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a few typos and added in the collection profile
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="369">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +233,18 @@
     <t>http://www.language-archives.org/REC/type-20020628.html#text/drama</t>
   </si>
   <si>
+    <t>txc:ElicitationTask</t>
+  </si>
+  <si>
+    <t>The collection protocol includes a task-based prompt to participants</t>
+  </si>
+  <si>
+    <t>"txc:CollectionProtocolTypeTerms"</t>
+  </si>
+  <si>
+    <t>ElicitationTask</t>
+  </si>
+  <si>
     <t>txc:Formulaic</t>
   </si>
   <si>
@@ -425,16 +437,13 @@
     <t>Syntactic</t>
   </si>
   <si>
-    <t>txc:Task</t>
-  </si>
-  <si>
-    <t>The collection protocol includes a task-based prompt to partipants</t>
-  </si>
-  <si>
-    <t>"txc:CollectionProtocolTypeTerms"</t>
-  </si>
-  <si>
-    <t>Task</t>
+    <t>txc:TextSelectionCriteria</t>
+  </si>
+  <si>
+    <t>A description of the criteria used to select texts in a collection</t>
+  </si>
+  <si>
+    <t>TextSelectionCriteria</t>
   </si>
   <si>
     <t>txc:Thesaurus</t>
@@ -510,7 +519,7 @@
     <t>txc:CollectionProtocolTypeTerms</t>
   </si>
   <si>
-    <t>"txc:Task"</t>
+    <t>["txc:ElicitationTask", "txc:TextSelectionCriteria"]</t>
   </si>
   <si>
     <t>txc:CommunicationGenreTerms</t>
@@ -787,6 +796,15 @@
   </si>
   <si>
     <t xml:space="preserve">This resource references another resource that describes it  such as a translation, transcription or other analysis </t>
+  </si>
+  <si>
+    <t>hasCollectionProtocol</t>
+  </si>
+  <si>
+    <t>txc:hasCollectionProtocol</t>
+  </si>
+  <si>
+    <t>This resource  was assembled or collected according to the linked protocol</t>
   </si>
   <si>
     <t>txc:hasDerivation</t>
@@ -1864,7 +1882,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -1944,7 +1962,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1955,94 +1973,94 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
       </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
       <c r="D7" t="s">
         <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2053,92 +2071,95 @@
       <c r="B11" t="s">
         <v>59</v>
       </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
-        <v>65</v>
-      </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
-        <v>96</v>
-      </c>
       <c r="D13" t="s">
         <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
       <c r="D14" t="s">
         <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
-        <v>101</v>
-      </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
       </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
@@ -2147,12 +2168,12 @@
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
@@ -2161,12 +2182,12 @@
         <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
@@ -2175,157 +2196,154 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C23" t="s">
-        <v>118</v>
-      </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>123</v>
       </c>
-      <c r="F24" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>125</v>
       </c>
       <c r="B25" t="s">
         <v>59</v>
       </c>
       <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
         <v>126</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>127</v>
       </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -2336,81 +2354,81 @@
         <v>139</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
         <v>140</v>
       </c>
-      <c r="F29" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" t="s">
         <v>143</v>
       </c>
-      <c r="D30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>144</v>
-      </c>
-      <c r="F30" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
         <v>19</v>
       </c>
       <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" t="s">
         <v>148</v>
       </c>
-      <c r="F31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>149</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
       </c>
+      <c r="C32" t="s">
+        <v>150</v>
+      </c>
       <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="F32" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
-        <v>152</v>
-      </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="E33" t="s">
         <v>153</v>
@@ -2427,10 +2445,27 @@
         <v>155</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2455,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -2463,86 +2498,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2553,7 +2588,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2567,13 +2602,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
@@ -2582,7 +2617,7 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
@@ -2591,540 +2626,531 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G8" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H8" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="G9" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I9" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I10" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J10" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F12" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="I12" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F13" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G13" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F14" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G14" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J14" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F15" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G15" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G16" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I16" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D17" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E17" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F17" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G17" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E18" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F18" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="G18" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
         <v>255</v>
       </c>
-      <c r="B19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D19" t="s">
-        <v>256</v>
-      </c>
       <c r="E19" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="F19" t="s">
+        <v>260</v>
+      </c>
+      <c r="G19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="s">
+        <v>262</v>
+      </c>
+      <c r="E20" t="s">
         <v>232</v>
       </c>
-      <c r="G19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>258</v>
-      </c>
-      <c r="E20" t="s">
-        <v>190</v>
-      </c>
       <c r="F20" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="G20" t="s">
-        <v>258</v>
-      </c>
-      <c r="I20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
+        <v>193</v>
       </c>
       <c r="F21" t="s">
+        <v>265</v>
+      </c>
+      <c r="G21" t="s">
         <v>264</v>
       </c>
-      <c r="G21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E22" t="s">
-        <v>190</v>
+        <v>269</v>
       </c>
       <c r="F22" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G22" t="s">
-        <v>266</v>
-      </c>
-      <c r="I22" t="s">
         <v>268</v>
       </c>
-      <c r="J22" t="s">
-        <v>269</v>
-      </c>
-      <c r="K22" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -3133,7 +3159,7 @@
         <v>272</v>
       </c>
       <c r="E23" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F23" t="s">
         <v>273</v>
@@ -3144,403 +3170,403 @@
       <c r="I23" t="s">
         <v>274</v>
       </c>
+      <c r="J23" t="s">
+        <v>275</v>
+      </c>
+      <c r="K23" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F24" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G24" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I24" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C25" t="s">
-        <v>279</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
+        <v>282</v>
+      </c>
+      <c r="E25" t="s">
+        <v>193</v>
+      </c>
+      <c r="F25" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" t="s">
+        <v>282</v>
+      </c>
+      <c r="I25" t="s">
         <v>280</v>
       </c>
-      <c r="E25" t="s">
-        <v>281</v>
-      </c>
-      <c r="F25" t="s">
-        <v>282</v>
-      </c>
-      <c r="G25" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>284</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" t="s">
+        <v>286</v>
+      </c>
+      <c r="E26" t="s">
+        <v>287</v>
+      </c>
+      <c r="F26" t="s">
+        <v>288</v>
+      </c>
+      <c r="G26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>290</v>
+      </c>
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="D26" t="s">
-        <v>285</v>
-      </c>
-      <c r="E26" t="s">
-        <v>286</v>
-      </c>
-      <c r="F26" t="s">
-        <v>287</v>
-      </c>
-      <c r="G26" t="s">
-        <v>285</v>
-      </c>
-      <c r="I26" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>289</v>
-      </c>
-      <c r="B27" t="s">
-        <v>180</v>
-      </c>
-      <c r="C27" t="s">
-        <v>182</v>
-      </c>
       <c r="D27" t="s">
-        <v>290</v>
+        <v>291</v>
+      </c>
+      <c r="E27" t="s">
+        <v>292</v>
+      </c>
+      <c r="F27" t="s">
+        <v>293</v>
       </c>
       <c r="G27" t="s">
-        <v>290</v>
-      </c>
-      <c r="H27" t="s">
         <v>291</v>
+      </c>
+      <c r="I27" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="D28" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G28" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H28" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>296</v>
-      </c>
-      <c r="E29" t="s">
-        <v>190</v>
-      </c>
-      <c r="F29" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G29" t="s">
-        <v>296</v>
-      </c>
-      <c r="I29" t="s">
-        <v>298</v>
-      </c>
-      <c r="J29" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F30" t="s">
+        <v>303</v>
+      </c>
+      <c r="G30" t="s">
         <v>302</v>
       </c>
-      <c r="G30" t="s">
-        <v>301</v>
-      </c>
       <c r="I30" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J30" t="s">
-        <v>304</v>
-      </c>
-      <c r="K30" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>306</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
         <v>307</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>193</v>
+      </c>
+      <c r="F31" t="s">
         <v>308</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
+        <v>307</v>
+      </c>
+      <c r="I31" t="s">
         <v>309</v>
       </c>
-      <c r="F31" t="s">
+      <c r="J31" t="s">
         <v>310</v>
       </c>
-      <c r="G31" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>313</v>
       </c>
       <c r="D32" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E32" t="s">
-        <v>190</v>
+        <v>315</v>
       </c>
       <c r="F32" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G32" t="s">
-        <v>312</v>
-      </c>
-      <c r="I32" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B33" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E33" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F33" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G33" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I33" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="E34" t="s">
+        <v>193</v>
       </c>
       <c r="F34" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G34" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="I34" t="s">
-        <v>322</v>
-      </c>
-      <c r="J34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>324</v>
-      </c>
-      <c r="E35" t="s">
-        <v>190</v>
+        <v>326</v>
       </c>
       <c r="F35" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G35" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="I35" t="s">
-        <v>326</v>
+        <v>328</v>
+      </c>
+      <c r="J35" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B36" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E36" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F36" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G36" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I36" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E37" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F37" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G37" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="I37" t="s">
-        <v>334</v>
-      </c>
-      <c r="J37" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C38" t="s">
         <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E38" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F38" t="s">
+        <v>339</v>
+      </c>
+      <c r="G38" t="s">
         <v>338</v>
       </c>
-      <c r="G38" t="s">
-        <v>337</v>
-      </c>
       <c r="I38" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J38" t="s">
-        <v>340</v>
-      </c>
-      <c r="K38" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>342</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
@@ -3549,7 +3575,7 @@
         <v>343</v>
       </c>
       <c r="E39" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F39" t="s">
         <v>344</v>
@@ -3560,45 +3586,45 @@
       <c r="I39" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>346</v>
+      </c>
+      <c r="K39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E40" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F40" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G40" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="I40" t="s">
-        <v>349</v>
-      </c>
-      <c r="J40" t="s">
-        <v>350</v>
-      </c>
-      <c r="K40" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>352</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
@@ -3607,7 +3633,7 @@
         <v>353</v>
       </c>
       <c r="E41" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F41" t="s">
         <v>354</v>
@@ -3618,57 +3644,89 @@
       <c r="I41" t="s">
         <v>355</v>
       </c>
+      <c r="J41" t="s">
+        <v>356</v>
+      </c>
+      <c r="K41" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E42" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F42" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G42" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="I42" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E43" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F43" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G43" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="I43" t="s">
-        <v>288</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>366</v>
+      </c>
+      <c r="B44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>367</v>
+      </c>
+      <c r="E44" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" t="s">
+        <v>368</v>
+      </c>
+      <c r="G44" t="s">
+        <v>367</v>
+      </c>
+      <c r="I44" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up and improved vocab
</commit_message>
<xml_diff>
--- a/ontology/ro-crate-metadata.xlsx
+++ b/ontology/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="391">
   <si>
     <t>Name</t>
   </si>
@@ -127,19 +127,19 @@
     <t>CollectionProtocol</t>
   </si>
   <si>
-    <t xml:space="preserve">Description of how this Object or Collection was obtained – such as strategy used for selecting orthographic text, or the prompts given to participants </t>
-  </si>
-  <si>
-    <t>txc:DerivedText</t>
-  </si>
-  <si>
-    <t>DerivedText</t>
+    <t xml:space="preserve">Description of how this Object or Collection was obtained – such as strategy used for selecting written source texts, or the prompts given to participants </t>
+  </si>
+  <si>
+    <t>txc:DerivedResource</t>
+  </si>
+  <si>
+    <t>DerivedResource</t>
   </si>
   <si>
     <t>http://www.language-archives.org/REC/type-20020628.html#text</t>
   </si>
   <si>
-    <t xml:space="preserve">A resource is derived from another resource, via some automated process, eg a downsampled video or an abstract of a text which  is not an analytical product </t>
+    <t>A resource is derived from another resource, via some automated process, eg a downsampled video or an abstract of a resource which  is not an annoation (description)</t>
   </si>
   <si>
     <t>txc:OrganizationBasedLicense</t>
@@ -184,13 +184,13 @@
     <t>[{"@id":"schema:Person"}, {"@id":"schema:Role"}]</t>
   </si>
   <si>
-    <t>txc:PrimaryText</t>
-  </si>
-  <si>
-    <t>PrimaryText</t>
-  </si>
-  <si>
-    <t>This is a primary resource: the object of study.   A text is defined as any primary resource or research material, such as a literary work, film, or recording of natural discourse</t>
+    <t>txc:PrimaryResource</t>
+  </si>
+  <si>
+    <t>PrimaryResource</t>
+  </si>
+  <si>
+    <t>This is a primary resource: the object of study, such as a literary work, film, or recording of natural discourse</t>
   </si>
   <si>
     <t>txc:Code</t>
@@ -205,7 +205,7 @@
     <t>CommunicationModeTerms</t>
   </si>
   <si>
-    <t>Code</t>
+    <t>Coded</t>
   </si>
   <si>
     <t>txc:Dialogue</t>
@@ -261,13 +261,16 @@
     <t>txc:Gesture</t>
   </si>
   <si>
+    <t>The resource contains non-linguistic gestural communication (ie not sign language)</t>
+  </si>
+  <si>
     <t>Gesture</t>
   </si>
   <si>
     <t>txc:Handwritten</t>
   </si>
   <si>
-    <t>The resource was written using a writing implement such as pen, pencil, brush or computer stylus</t>
+    <t>The resource was written using a writing implement such as pen, pencil, brush or computer stylus  (From Nyingarn - TODO check this)</t>
   </si>
   <si>
     <t>Handwritten</t>
@@ -276,7 +279,7 @@
     <t>txc:Informational</t>
   </si>
   <si>
-    <t>SIMON – TODO</t>
+    <t xml:space="preserve"> Discourse whose primary purpose is to inform the reader about the natural or social world.</t>
   </si>
   <si>
     <t>Informational</t>
@@ -304,94 +307,148 @@
     <t>http://www.language-archives.org/REC/type-20020628.html#Lexicon</t>
   </si>
   <si>
-    <t>txc:LinguisticDescription</t>
-  </si>
-  <si>
-    <t>LinguisticDescription</t>
-  </si>
-  <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#description</t>
-  </si>
-  <si>
     <t>txc:Ludic</t>
   </si>
   <si>
+    <t>Ludic discourse is language whose primary function is to be part of play, or a style of speech that involves a creative manipulation of the structures of the language. Examples of ludic discourse are play languages, jokes, secret languages, and speech disguises.</t>
+  </si>
+  <si>
     <t>Ludic</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/ludic</t>
+  </si>
+  <si>
     <t>txc:Narrative</t>
   </si>
   <si>
-    <t>A monologic discourse which represents temporally organized events.</t>
+    <t>A monologic discourse which represents temporally organized events. Types of narratives include historical, traditional, and personal narratives, myths, folktales, fables, and humorous stories.</t>
   </si>
   <si>
     <t>Narrative</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/narrative</t>
+  </si>
+  <si>
     <t>txc:Oratory</t>
   </si>
   <si>
+    <t>The art of public speaking, or of speaking eloquently according to rules or conventions. Examples of oratory include sermons, lectures, political speeches, and invocations.</t>
+  </si>
+  <si>
     <t>Oratory</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/orratory</t>
+  </si>
+  <si>
+    <t>txc:Orthographic</t>
+  </si>
+  <si>
+    <t>The resource contains annotations using  orthography (a writing ssytem) as opposed to a coded analysis such as a phonetic transcription</t>
+  </si>
+  <si>
+    <t>Orthographic</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/orthographic</t>
+  </si>
+  <si>
     <t>txc:Orthography</t>
   </si>
   <si>
     <t>The resource contains written material using a standard or conventional orthography with conventions for punctuation, capitalization etc</t>
   </si>
   <si>
-    <t>Orthography</t>
+    <t>WrittenLanguage</t>
   </si>
   <si>
     <t>txc:PartOfSpeech</t>
   </si>
   <si>
+    <t>TODO - Olac definitons are circular</t>
+  </si>
+  <si>
     <t>PartOfSpeech</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/part-of-spoeech</t>
+  </si>
+  <si>
     <t>txc:Phonemic</t>
   </si>
   <si>
     <t>Phonemic</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/phonemic</t>
+  </si>
+  <si>
     <t>txc:Phonetic</t>
   </si>
   <si>
     <t>Phonetic</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/phonetic</t>
+  </si>
+  <si>
     <t>txc:Phonological</t>
   </si>
   <si>
     <t>Phonological</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/phonological</t>
+  </si>
+  <si>
     <t>txc:Procedural</t>
   </si>
   <si>
+    <t>An explanation or description of a method, process, or situation having ordered steps.</t>
+  </si>
+  <si>
     <t>Procedural</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/procedural</t>
+  </si>
+  <si>
     <t>txc:Prosodic</t>
   </si>
   <si>
     <t>Prosodic</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/prosodic</t>
+  </si>
+  <si>
     <t>txc:Report</t>
   </si>
   <si>
+    <t>A factual account of some event or circumstance.</t>
+  </si>
+  <si>
     <t>Report</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/report</t>
+  </si>
+  <si>
     <t>txc:Semantic</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>The resource contains annotations of the meaning of another resource</t>
+  </si>
+  <si>
+    <t>txc:DerivedTextTypeTerms</t>
   </si>
   <si>
     <t>Semantic</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/semantic</t>
   </si>
   <si>
     <t>txc:Session</t>
@@ -419,22 +476,28 @@
     <t>Song</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#text/singing</t>
+  </si>
+  <si>
     <t>txc:Speech</t>
   </si>
   <si>
-    <t>This resource contains a video recording of  sign language</t>
-  </si>
-  <si>
-    <t>Speech</t>
+    <t>This resource contains  spoken language</t>
+  </si>
+  <si>
+    <t>SpokenLanguage</t>
   </si>
   <si>
     <t>txc:Syntactic</t>
   </si>
   <si>
-    <t>The resource contains annotation or other analysis describing  the syntactic structure of a PrimaryText</t>
+    <t>The resource contains annotation or analysis describing  the syntactic structure of another resource</t>
   </si>
   <si>
     <t>Syntactic</t>
+  </si>
+  <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#description/syntactic</t>
   </si>
   <si>
     <t>txc:TextSelectionCriteria</t>
@@ -456,7 +519,7 @@
     <t>Thesaurus</t>
   </si>
   <si>
-    <t>http://www.language-archives.org/REC/type-20020628.html#text/singing</t>
+    <t>http://www.language-archives.org/REC/type-20020628.html#lexicon/thesaurus</t>
   </si>
   <si>
     <t>txc:TimeAligned</t>
@@ -468,24 +531,30 @@
     <t>TimeAligned</t>
   </si>
   <si>
+    <t>txc:Transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The resource contains a transcription, which  is a written (orthographic) or coded  representation of an audio or visual signal. </t>
+  </si>
+  <si>
+    <t>Transcription</t>
+  </si>
+  <si>
     <t>http://www.language-archives.org/REC/type-20020628.html#transcription</t>
   </si>
   <si>
-    <t>txc:Transcription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The resource contains a transcription, which  is a written (orthographic) or coded  representation of an audio or visual signal. </t>
-  </si>
-  <si>
-    <t>Transcription</t>
-  </si>
-  <si>
     <t>txc:Translation</t>
   </si>
   <si>
+    <t>The resource has been translated from one natual language to another</t>
+  </si>
+  <si>
     <t>Translation</t>
   </si>
   <si>
+    <t>http://www.language-archives.org/REC/type-20020628.html#annotation/translation</t>
+  </si>
+  <si>
     <t>txc:Typeset</t>
   </si>
   <si>
@@ -498,7 +567,7 @@
     <t>txc:Typewritten</t>
   </si>
   <si>
-    <t>The annotation has time-alignement with the PrimaryText</t>
+    <t>The resource contains text produced on a tpyewriter (From Nyingarn - TODO check this)</t>
   </si>
   <si>
     <t>Typewritten</t>
@@ -534,13 +603,10 @@
     <t>txc:CommunicationModeTerms</t>
   </si>
   <si>
-    <t>["txc:Speech", "txc:Orthography", "txc:Singing", "txc:Gesture"]</t>
+    <t>["txc:SpokenLanguage", "txc:WrittenLanguage", "txc:Song", "txc:Gesture", "txc:SignLanguage"]</t>
   </si>
   <si>
     <t>ModalityTerms</t>
-  </si>
-  <si>
-    <t>txc:DerivedTextTypeTerms</t>
   </si>
   <si>
     <t>["txc:Phonemic", "txc:Phonetic", "txc:Phonological", "txc:Syntactic", "txc:Translation", "txc:Semantic", "txc:Transcription", "txc:TimeAligned", "txc:Prosodic"]</t>
@@ -2006,466 +2072,544 @@
       <c r="B7" t="s">
         <v>59</v>
       </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
       <c r="D7" t="s">
         <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
       </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
       <c r="D13" t="s">
         <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
         <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
       </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
       </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
       </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
       <c r="D21" t="s">
         <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>59</v>
       </c>
+      <c r="C22" t="s">
+        <v>115</v>
+      </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
         <v>59</v>
       </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
       <c r="D23" t="s">
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="F23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
         <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="D26" t="s">
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
         <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>157</v>
+      </c>
+      <c r="F28" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="D30" t="s">
         <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D31" t="s">
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="F32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
       </c>
+      <c r="C33" t="s">
+        <v>174</v>
+      </c>
       <c r="D33" t="s">
         <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
+        <v>175</v>
+      </c>
+      <c r="F33" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2490,7 +2634,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -2498,86 +2642,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2602,13 +2746,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
@@ -2617,7 +2761,7 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
@@ -2626,165 +2770,165 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="H3" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="G5" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="I5" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="G6" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="F7" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="G7" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="H7" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="G8" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="H8" t="s">
         <v>73</v>
@@ -2792,941 +2936,941 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="E9" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F9" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="G9" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="I9" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="J9" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="K9" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="E10" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="G10" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="I10" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="J10" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="I11" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="E12" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F12" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="I12" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="E13" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="F13" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="G13" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="E14" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="G14" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="I14" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="J14" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="F15" t="s">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="G15" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="G16" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="I16" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="J16" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C17" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="D17" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="E17" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="F17" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="G17" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="D18" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="E18" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="G18" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="E19" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="F19" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="G19" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="F20" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="G20" t="s">
-        <v>262</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="G21" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="I21" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="E22" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="F22" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="G22" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="E23" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="G23" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="I23" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="J23" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="K23" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="E24" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F24" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="G24" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="I24" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>281</v>
+        <v>303</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="E25" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F25" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="G25" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="I25" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>284</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="D26" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="E26" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="F26" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="G26" t="s">
-        <v>289</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>312</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>291</v>
+        <v>313</v>
       </c>
       <c r="E27" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="F27" t="s">
-        <v>293</v>
+        <v>315</v>
       </c>
       <c r="G27" t="s">
-        <v>291</v>
+        <v>313</v>
       </c>
       <c r="I27" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="D28" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="G28" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="H28" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="G29" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="H29" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="E30" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F30" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="G30" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="I30" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="J30" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="E31" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="G31" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="I31" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="J31" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="K31" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C32" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="D32" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="E32" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
       <c r="F32" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="G32" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="E33" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F33" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="G33" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="I33" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="E34" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F34" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
       <c r="G34" t="s">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="I34" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="B35" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="F35" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="G35" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="I35" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="J35" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="E36" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F36" t="s">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="G36" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="I36" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="E37" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F37" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
       <c r="G37" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="I37" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="B38" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
         <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="E38" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F38" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="G38" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="I38" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="J38" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F39" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="G39" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="I39" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="J39" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="K39" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="E40" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F40" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="G40" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="I40" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="E41" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F41" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="G41" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="I41" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="J41" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="K41" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
       <c r="B42" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
       <c r="E42" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F42" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
       <c r="G42" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
       <c r="I42" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>362</v>
+        <v>384</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C43" t="s">
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="E43" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F43" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="G43" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="I43" t="s">
-        <v>365</v>
+        <v>387</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="C44" t="s">
         <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="E44" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="F44" t="s">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="G44" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="I44" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>